<commit_message>
Update laser worksheet template tospecify YAML, not SYNC-file
</commit_message>
<xml_diff>
--- a/docs/templates/template_taini_worksheet_laser.xlsx
+++ b/docs/templates/template_taini_worksheet_laser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ye2svr02\BEHAV4\People\John Huxter\Projects\Platform_Laser_ERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yex7906\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248EC8FE-FE02-420D-941F-598AC9101AA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832E8C5C-44B5-43A2-BFEA-3A4F4D1432CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="630" windowWidth="19875" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExperimentalWorksheet_v2_sample" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    eg: 20191003-000_39067.sync</t>
+    eg: TAINI_D001_45225-2019_11_27-0000_configuration.yaml</t>
       </text>
     </comment>
     <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
@@ -161,16 +161,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>DOSSIER_IDS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 4 mm </t>
   </si>
   <si>
     <t xml:space="preserve"> 4 ms</t>
-  </si>
-  <si>
-    <t>SYNC_FILE=</t>
   </si>
   <si>
     <t>BLOCK#3</t>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t>"x"tot:</t>
+  </si>
+  <si>
+    <t>YAML_FILE=</t>
+  </si>
+  <si>
+    <t>SUBJECT_IDS</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -487,11 +487,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -500,9 +502,37 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin">
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -515,7 +545,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -524,67 +554,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -594,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -667,24 +643,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -700,37 +669,46 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,7 +1095,7 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="B1" dT="2019-10-30T15:31:27.28" personId="{9845AEAD-3964-44A4-8D42-B75195D6D277}" id="{80DAF895-A748-4002-A930-4527E3C67DC1}">
-    <text>eg: 20191003-000_39067.sync</text>
+    <text>eg: TAINI_D001_45225-2019_11_27-0000_configuration.yaml</text>
   </threadedComment>
   <threadedComment ref="B2" dT="2019-10-30T15:30:23.39" personId="{9845AEAD-3964-44A4-8D42-B75195D6D277}" id="{434AAF0A-C372-4BCE-ACF6-504D47EBBDC7}">
     <text>eg:  IA14DF819 (John Huxter)</text>
@@ -1139,85 +1117,85 @@
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="5.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="1" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="37" t="s">
+    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-    </row>
-    <row r="7" spans="1:9" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="6" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="26">
@@ -1244,9 +1222,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>29</v>
+    <row r="8" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -1263,41 +1241,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>20</v>
+    <row r="9" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>1</v>
@@ -1324,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>1</v>
       </c>
@@ -1349,7 +1327,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>2</v>
       </c>
@@ -1374,7 +1352,7 @@
       </c>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>3</v>
       </c>
@@ -1399,7 +1377,7 @@
       </c>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>4</v>
       </c>
@@ -1424,7 +1402,7 @@
       </c>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>5</v>
       </c>
@@ -1449,7 +1427,7 @@
       </c>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>6</v>
       </c>
@@ -1474,7 +1452,7 @@
       </c>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>7</v>
       </c>
@@ -1499,7 +1477,7 @@
       </c>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>8</v>
       </c>
@@ -1524,7 +1502,7 @@
       </c>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>9</v>
       </c>
@@ -1549,7 +1527,7 @@
       </c>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>10</v>
       </c>
@@ -1577,7 +1555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>11</v>
       </c>
@@ -1602,7 +1580,7 @@
       </c>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>12</v>
       </c>
@@ -1621,33 +1599,33 @@
         <v>47</v>
       </c>
       <c r="G24" s="19"/>
-      <c r="H24" s="42">
+      <c r="H24" s="34">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="I24" s="43"/>
-    </row>
-    <row r="25" spans="1:11" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H25" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="45">
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="1:11" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="37">
         <f>SUMPRODUCT(LEN(C13:I24)-LEN(SUBSTITUTE(UPPER(C13:I24),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="36"/>
-    </row>
-    <row r="27" spans="1:11" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="33"/>
+    </row>
+    <row r="27" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>1</v>
@@ -1674,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22">
         <v>13</v>
       </c>
@@ -1699,7 +1677,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>14</v>
       </c>
@@ -1724,7 +1702,7 @@
       </c>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>15</v>
       </c>
@@ -1749,7 +1727,7 @@
       </c>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>16</v>
       </c>
@@ -1774,7 +1752,7 @@
       </c>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>17</v>
       </c>
@@ -1799,7 +1777,7 @@
       </c>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>18</v>
       </c>
@@ -1824,7 +1802,7 @@
       </c>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>19</v>
       </c>
@@ -1849,7 +1827,7 @@
       </c>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>20</v>
       </c>
@@ -1874,7 +1852,7 @@
       </c>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>21</v>
       </c>
@@ -1899,7 +1877,7 @@
       </c>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>22</v>
       </c>
@@ -1924,7 +1902,7 @@
       </c>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>23</v>
       </c>
@@ -1949,7 +1927,7 @@
       </c>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>24</v>
       </c>
@@ -1974,27 +1952,27 @@
       </c>
       <c r="I39" s="21"/>
     </row>
-    <row r="40" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H40" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="45">
+    <row r="40" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" s="37">
         <f>SUMPRODUCT(LEN(C28:I39)-LEN(SUBSTITUTE(UPPER(C28:I39),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="36"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="33"/>
+    </row>
+    <row r="42" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>1</v>
@@ -2021,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A43" s="22">
         <v>25</v>
       </c>
@@ -2046,7 +2024,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>26</v>
       </c>
@@ -2071,7 +2049,7 @@
       </c>
       <c r="I44" s="18"/>
     </row>
-    <row r="45" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>27</v>
       </c>
@@ -2096,7 +2074,7 @@
       </c>
       <c r="I45" s="18"/>
     </row>
-    <row r="46" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>28</v>
       </c>
@@ -2121,7 +2099,7 @@
       </c>
       <c r="I46" s="18"/>
     </row>
-    <row r="47" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>29</v>
       </c>
@@ -2146,7 +2124,7 @@
       </c>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>30</v>
       </c>
@@ -2171,7 +2149,7 @@
       </c>
       <c r="I48" s="18"/>
     </row>
-    <row r="49" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>31</v>
       </c>
@@ -2196,7 +2174,7 @@
       </c>
       <c r="I49" s="18"/>
     </row>
-    <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>32</v>
       </c>
@@ -2221,7 +2199,7 @@
       </c>
       <c r="I50" s="18"/>
     </row>
-    <row r="51" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>33</v>
       </c>
@@ -2246,7 +2224,7 @@
       </c>
       <c r="I51" s="18"/>
     </row>
-    <row r="52" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>34</v>
       </c>
@@ -2271,7 +2249,7 @@
       </c>
       <c r="I52" s="18"/>
     </row>
-    <row r="53" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>35</v>
       </c>
@@ -2296,7 +2274,7 @@
       </c>
       <c r="I53" s="18"/>
     </row>
-    <row r="54" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>36</v>
       </c>
@@ -2321,27 +2299,27 @@
       </c>
       <c r="I54" s="21"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H55" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I55" s="45">
+    <row r="55" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H55" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" s="37">
         <f>SUMPRODUCT(LEN(C43:I54)-LEN(SUBSTITUTE(UPPER(C43:I54),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="36"/>
-    </row>
-    <row r="64" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="33"/>
+    </row>
+    <row r="64" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>1</v>
@@ -2368,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A65" s="25">
         <v>37</v>
       </c>
@@ -2393,7 +2371,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>38</v>
       </c>
@@ -2418,7 +2396,7 @@
       </c>
       <c r="I66" s="18"/>
     </row>
-    <row r="67" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="22">
         <v>39</v>
       </c>
@@ -2443,7 +2421,7 @@
       </c>
       <c r="I67" s="18"/>
     </row>
-    <row r="68" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>40</v>
       </c>
@@ -2468,7 +2446,7 @@
       </c>
       <c r="I68" s="18"/>
     </row>
-    <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="22">
         <v>41</v>
       </c>
@@ -2493,7 +2471,7 @@
       </c>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>42</v>
       </c>
@@ -2518,7 +2496,7 @@
       </c>
       <c r="I70" s="18"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="22">
         <v>43</v>
       </c>
@@ -2543,7 +2521,7 @@
       </c>
       <c r="I71" s="18"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>44</v>
       </c>
@@ -2568,7 +2546,7 @@
       </c>
       <c r="I72" s="18"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="22">
         <v>45</v>
       </c>
@@ -2593,7 +2571,7 @@
       </c>
       <c r="I73" s="18"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>46</v>
       </c>
@@ -2618,7 +2596,7 @@
       </c>
       <c r="I74" s="18"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="22">
         <v>47</v>
       </c>
@@ -2643,7 +2621,7 @@
       </c>
       <c r="I75" s="18"/>
     </row>
-    <row r="76" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <v>48</v>
       </c>
@@ -2668,27 +2646,27 @@
       </c>
       <c r="I76" s="21"/>
     </row>
-    <row r="77" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H77" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I77" s="45">
+    <row r="77" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H77" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="37">
         <f>SUMPRODUCT(LEN(C65:I76)-LEN(SUBSTITUTE(UPPER(C65:I76),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B78" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="36"/>
-    </row>
-    <row r="79" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="33"/>
+    </row>
+    <row r="79" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>1</v>
@@ -2715,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A80" s="25">
         <v>49</v>
       </c>
@@ -2740,7 +2718,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>50</v>
       </c>
@@ -2765,7 +2743,7 @@
       </c>
       <c r="I81" s="18"/>
     </row>
-    <row r="82" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="22">
         <v>51</v>
       </c>
@@ -2790,7 +2768,7 @@
       </c>
       <c r="I82" s="18"/>
     </row>
-    <row r="83" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>52</v>
       </c>
@@ -2815,7 +2793,7 @@
       </c>
       <c r="I83" s="18"/>
     </row>
-    <row r="84" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="22">
         <v>53</v>
       </c>
@@ -2840,7 +2818,7 @@
       </c>
       <c r="I84" s="18"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>54</v>
       </c>
@@ -2865,7 +2843,7 @@
       </c>
       <c r="I85" s="18"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="22">
         <v>55</v>
       </c>
@@ -2890,7 +2868,7 @@
       </c>
       <c r="I86" s="18"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>56</v>
       </c>
@@ -2915,7 +2893,7 @@
       </c>
       <c r="I87" s="18"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="22">
         <v>57</v>
       </c>
@@ -2940,7 +2918,7 @@
       </c>
       <c r="I88" s="18"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>58</v>
       </c>
@@ -2965,7 +2943,7 @@
       </c>
       <c r="I89" s="18"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="22">
         <v>59</v>
       </c>
@@ -2990,7 +2968,7 @@
       </c>
       <c r="I90" s="18"/>
     </row>
-    <row r="91" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9">
         <v>60</v>
       </c>
@@ -3015,27 +2993,27 @@
       </c>
       <c r="I91" s="21"/>
     </row>
-    <row r="92" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H92" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I92" s="45">
+    <row r="92" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H92" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I92" s="37">
         <f>SUMPRODUCT(LEN(C80:I91)-LEN(SUBSTITUTE(UPPER(C80:I91),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B93" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="36"/>
-    </row>
-    <row r="94" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="33"/>
+    </row>
+    <row r="94" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>1</v>
@@ -3062,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A95" s="25">
         <v>61</v>
       </c>
@@ -3087,7 +3065,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>62</v>
       </c>
@@ -3112,7 +3090,7 @@
       </c>
       <c r="I96" s="18"/>
     </row>
-    <row r="97" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="22">
         <v>63</v>
       </c>
@@ -3137,7 +3115,7 @@
       </c>
       <c r="I97" s="18"/>
     </row>
-    <row r="98" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>64</v>
       </c>
@@ -3162,7 +3140,7 @@
       </c>
       <c r="I98" s="18"/>
     </row>
-    <row r="99" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="22">
         <v>65</v>
       </c>
@@ -3187,7 +3165,7 @@
       </c>
       <c r="I99" s="18"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>66</v>
       </c>
@@ -3212,7 +3190,7 @@
       </c>
       <c r="I100" s="18"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="22">
         <v>67</v>
       </c>
@@ -3237,7 +3215,7 @@
       </c>
       <c r="I101" s="18"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>68</v>
       </c>
@@ -3262,7 +3240,7 @@
       </c>
       <c r="I102" s="18"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="22">
         <v>69</v>
       </c>
@@ -3287,7 +3265,7 @@
       </c>
       <c r="I103" s="18"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>70</v>
       </c>
@@ -3312,7 +3290,7 @@
       </c>
       <c r="I104" s="18"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="22">
         <v>71</v>
       </c>
@@ -3337,7 +3315,7 @@
       </c>
       <c r="I105" s="18"/>
     </row>
-    <row r="106" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9">
         <v>72</v>
       </c>
@@ -3362,24 +3340,24 @@
       </c>
       <c r="I106" s="21"/>
     </row>
-    <row r="107" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H107" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I107" s="45">
+    <row r="107" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H107" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I107" s="37">
         <f>SUMPRODUCT(LEN(C95:I106)-LEN(SUBSTITUTE(UPPER(C95:I106),"X","")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>17</v>
       </c>
@@ -3387,7 +3365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>14</v>
       </c>
@@ -3395,7 +3373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>16</v>
       </c>
@@ -3403,27 +3381,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C118" s="1" t="s">
         <v>19</v>
       </c>
@@ -3435,7 +3413,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="H13:I24 H28:I39 H43:I54">
     <cfRule type="expression" dxfId="13" priority="16">

</xml_diff>

<commit_message>
xs-TAINI-laser1: new script for building trials from laser-worksheet - replaces xs-TAINI-laser0 and xs-TAINI-sheet2plan template_taini_worksheet_laser.xlsx: update comments
</commit_message>
<xml_diff>
--- a/docs/templates/template_taini_worksheet_laser.xlsx
+++ b/docs/templates/template_taini_worksheet_laser.xlsx
@@ -39,7 +39,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,64 +48,6 @@
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">This sheet assumes up to 4 subjects are run at a time, in separate boxes arranged left-to-right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">The unique ID for the subject in each box for this recording session.
-NOTE: Leave the field completely blank to grey-out the column and adjust the anticipated stimulus-talley. 
-NOTE: empty boxes should always be on the right for the stimulus-talley to work correctly .
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This sheet assumes each subject should get a block of 12 stimuli before a break, ending the block. 
-NOTE: a new block does not represent a new recording. If you start a new recording, you need to generate another worksheet.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">The cumulative number of trials (stimuli) delivered to each subject</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The  TAINI config .yaml file corresponding to this recording session
 Example:
@@ -123,6 +65,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Optional name of the experimenter.</t>
         </r>
@@ -138,7 +81,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The date this session was recorded. Example:
+          <t xml:space="preserve">The date this session was recorded. Format: dd/mm/yyy. Example:
 25/12/2020</t>
         </r>
       </text>
@@ -151,6 +94,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The laser spot size
 Example: 4 mm</t>
@@ -165,13 +109,14 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The laser pulse duration
 Example: 4ms</t>
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,9 +126,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The cumulative number of trials (good stimuli) in this block, not counting “misses” (X’s)
-NOTE: adjusted according to whether some boxes are empty.
-NOTE: only accurate if the empty boxes are on the right!</t>
+          <t xml:space="preserve">Numeric values, must be greater than zero. 
+Leave blank to grey-out the box. 
+Empty boxes should be the rightmost for the stim-counts in this table to be accurate
+</t>
         </r>
       </text>
     </comment>
@@ -198,119 +144,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Enter the stimulus strength for this block of trials. Example: 1.50
-NOTE: Leaving this blank will mark the black as unused during data processing</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">For each good trial, enter the stimulated paw (BL, BR, FL, or FR) and the  response (1-4) 
-Also enter one "x" for each “miss”, where a  sync pulse was generated but no paw was stimulated, for whatever reason. 
-Example: two misses, then left-back paw, and  response 4: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-          </rPr>
-          <t xml:space="preserve">xx LB 4
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <u val="single"/>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Response codes: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">0: no movement
-1: head turning, including shaking or elevating the head
-2: flinching, that is, a small abrupt body jerking movement
-3: withdrawal, involving paw retraction from the nociceptive stimulus
-4: licking the stimulated body territory and whole-body movement
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Use one sheet per TAINI recording. 
-Assumes up to 4 subjects run at a time, with a sync-pulse generated for every stimulus delivered to either subject. 
-Assumes trials are run in blocks of 12 per animal (up to 48 total) before a break, but with TAINI data-acquisition  uninterrupted between blocks. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">NOTE</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val=""/>
-            <family val="1"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">: it’s good practice to print this template and fill it out in pen and paper during the actual recording session. Pen and paper is less prone to accidental deletion of data
-At the end of the session, scan the paper original and transcribe the data into a digital copy of the worksheet.
-Name the digital copy according to the date and session-number matching the TAINI configuration (.yaml) file
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Tally of missed trials (X’s) - add this to the total trials to get the expected number of sync pulses for this block </t>
+NOTE: set to “audio” to specify that stimuli were auditory – assumes all subjects get all stimuli
+NOTE: Leaving this blank will mark the block as unused during data processing</t>
         </r>
       </text>
     </comment>
@@ -327,7 +162,7 @@
     <t xml:space="preserve">refer to digital comments in this sheet for instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">YAML_FILE=</t>
+    <t xml:space="preserve">CONFIG_FILE=</t>
   </si>
   <si>
     <t xml:space="preserve">EXPERIMENTER=</t>
@@ -471,7 +306,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -529,44 +364,6 @@
       <color rgb="FFBFBFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val=""/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <u val="single"/>
-      <sz val="9"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -764,7 +561,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -777,10 +574,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -829,10 +622,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -853,10 +642,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -897,10 +682,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -913,10 +694,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -944,10 +721,6 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1136,19 +909,19 @@
   </sheetPr>
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.18"/>
@@ -1158,14 +931,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
+      <c r="I1" s="3"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1176,17 +942,11 @@
       <c r="R1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="0"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="3"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -1197,334 +957,334 @@
       <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="16" t="n">
         <f aca="false">SUM(C9,E9,G9,I9)</f>
         <v>4</v>
       </c>
-      <c r="C9" s="19" t="n">
+      <c r="C9" s="17" t="n">
         <f aca="false">IF(SUBJECT1&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="n">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17" t="n">
         <f aca="false">IF(SUBJECT2&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="n">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="n">
         <f aca="false">IF(SUBJECT3&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19" t="n">
+      <c r="H9" s="17"/>
+      <c r="I9" s="17" t="n">
         <f aca="false">IF(SUBJECT4&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="20" t="n">
+      <c r="D10" s="19"/>
+      <c r="E10" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="20" t="n">
+      <c r="F10" s="19"/>
+      <c r="G10" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="I10" s="20" t="n">
+      <c r="I10" s="18" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="22"/>
+      <c r="G11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="22"/>
+      <c r="I11" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="26" t="s">
         <v>17</v>
       </c>
       <c r="S14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="n">
+      <c r="A15" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="31" t="n">
+      <c r="B15" s="28" t="n">
         <f aca="false">(A15-1)*NBOXES+LBOX1</f>
         <v>1</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="31" t="n">
+      <c r="C15" s="29"/>
+      <c r="D15" s="28" t="n">
         <f aca="false">(A15-1)*NBOXES+LBOX2</f>
         <v>2</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31" t="n">
+      <c r="E15" s="29"/>
+      <c r="F15" s="28" t="n">
         <f aca="false">(A15-1)*NBOXES+LBOX3</f>
         <v>3</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="31" t="n">
+      <c r="G15" s="29"/>
+      <c r="H15" s="28" t="n">
         <f aca="false">(A15-1)*NBOXES+LBOX4</f>
         <v>4</v>
       </c>
-      <c r="I15" s="33"/>
+      <c r="I15" s="29"/>
       <c r="L15" s="0"/>
       <c r="R15" s="0"/>
       <c r="S15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="n">
+      <c r="A16" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="35" t="n">
+      <c r="B16" s="31" t="n">
         <f aca="false">(A16-1)*NBOXES+LBOX1</f>
         <v>5</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="35" t="n">
+      <c r="C16" s="32"/>
+      <c r="D16" s="31" t="n">
         <f aca="false">(A16-1)*NBOXES+LBOX2</f>
         <v>6</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="35" t="n">
+      <c r="E16" s="32"/>
+      <c r="F16" s="31" t="n">
         <f aca="false">(A16-1)*NBOXES+LBOX3</f>
         <v>7</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="35" t="n">
+      <c r="G16" s="32"/>
+      <c r="H16" s="31" t="n">
         <f aca="false">(A16-1)*NBOXES+LBOX4</f>
         <v>8</v>
       </c>
-      <c r="I16" s="37"/>
+      <c r="I16" s="32"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="n">
+      <c r="A17" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="B17" s="35" t="n">
+      <c r="B17" s="31" t="n">
         <f aca="false">(A17-1)*NBOXES+LBOX1</f>
         <v>9</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="35" t="n">
+      <c r="C17" s="32"/>
+      <c r="D17" s="31" t="n">
         <f aca="false">(A17-1)*NBOXES+LBOX2</f>
         <v>10</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="35" t="n">
+      <c r="E17" s="32"/>
+      <c r="F17" s="31" t="n">
         <f aca="false">(A17-1)*NBOXES+LBOX3</f>
         <v>11</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="35" t="n">
+      <c r="G17" s="32"/>
+      <c r="H17" s="31" t="n">
         <f aca="false">(A17-1)*NBOXES+LBOX4</f>
         <v>12</v>
       </c>
-      <c r="I17" s="37"/>
+      <c r="I17" s="32"/>
       <c r="L17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="n">
+      <c r="A18" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="B18" s="35" t="n">
+      <c r="B18" s="31" t="n">
         <f aca="false">(A18-1)*NBOXES+LBOX1</f>
         <v>13</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="35" t="n">
+      <c r="C18" s="32"/>
+      <c r="D18" s="31" t="n">
         <f aca="false">(A18-1)*NBOXES+LBOX2</f>
         <v>14</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="35" t="n">
+      <c r="E18" s="32"/>
+      <c r="F18" s="31" t="n">
         <f aca="false">(A18-1)*NBOXES+LBOX3</f>
         <v>15</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="35" t="n">
+      <c r="G18" s="32"/>
+      <c r="H18" s="31" t="n">
         <f aca="false">(A18-1)*NBOXES+LBOX4</f>
         <v>16</v>
       </c>
-      <c r="I18" s="37"/>
+      <c r="I18" s="32"/>
       <c r="K18" s="0"/>
       <c r="R18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="n">
+      <c r="A19" s="30" t="n">
         <v>5</v>
       </c>
-      <c r="B19" s="35" t="n">
+      <c r="B19" s="31" t="n">
         <f aca="false">(A19-1)*NBOXES+LBOX1</f>
         <v>17</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="35" t="n">
+      <c r="C19" s="32"/>
+      <c r="D19" s="31" t="n">
         <f aca="false">(A19-1)*NBOXES+LBOX2</f>
         <v>18</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="35" t="n">
+      <c r="E19" s="32"/>
+      <c r="F19" s="31" t="n">
         <f aca="false">(A19-1)*NBOXES+LBOX3</f>
         <v>19</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="35" t="n">
+      <c r="G19" s="32"/>
+      <c r="H19" s="31" t="n">
         <f aca="false">(A19-1)*NBOXES+LBOX4</f>
         <v>20</v>
       </c>
-      <c r="I19" s="37"/>
+      <c r="I19" s="32"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="n">
+      <c r="A20" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="B20" s="35" t="n">
+      <c r="B20" s="31" t="n">
         <f aca="false">(A20-1)*NBOXES+LBOX1</f>
         <v>21</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="35" t="n">
+      <c r="C20" s="32"/>
+      <c r="D20" s="31" t="n">
         <f aca="false">(A20-1)*NBOXES+LBOX2</f>
         <v>22</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="35" t="n">
+      <c r="E20" s="32"/>
+      <c r="F20" s="31" t="n">
         <f aca="false">(A20-1)*NBOXES+LBOX3</f>
         <v>23</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="35" t="n">
+      <c r="G20" s="32"/>
+      <c r="H20" s="31" t="n">
         <f aca="false">(A20-1)*NBOXES+LBOX4</f>
         <v>24</v>
       </c>
-      <c r="I20" s="37"/>
+      <c r="I20" s="32"/>
       <c r="M20" s="0"/>
       <c r="N20" s="0"/>
       <c r="O20" s="0"/>
@@ -1534,84 +1294,84 @@
       <c r="S20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="n">
+      <c r="A21" s="30" t="n">
         <v>7</v>
       </c>
-      <c r="B21" s="35" t="n">
+      <c r="B21" s="31" t="n">
         <f aca="false">(A21-1)*NBOXES+LBOX1</f>
         <v>25</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="35" t="n">
+      <c r="C21" s="32"/>
+      <c r="D21" s="31" t="n">
         <f aca="false">(A21-1)*NBOXES+LBOX2</f>
         <v>26</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="35" t="n">
+      <c r="E21" s="32"/>
+      <c r="F21" s="31" t="n">
         <f aca="false">(A21-1)*NBOXES+LBOX3</f>
         <v>27</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="35" t="n">
+      <c r="G21" s="32"/>
+      <c r="H21" s="31" t="n">
         <f aca="false">(A21-1)*NBOXES+LBOX4</f>
         <v>28</v>
       </c>
-      <c r="I21" s="37"/>
+      <c r="I21" s="32"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
       <c r="O21" s="0"/>
       <c r="P21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34" t="n">
+      <c r="A22" s="30" t="n">
         <v>8</v>
       </c>
-      <c r="B22" s="35" t="n">
+      <c r="B22" s="31" t="n">
         <f aca="false">(A22-1)*NBOXES+LBOX1</f>
         <v>29</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="35" t="n">
+      <c r="C22" s="32"/>
+      <c r="D22" s="31" t="n">
         <f aca="false">(A22-1)*NBOXES+LBOX2</f>
         <v>30</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="35" t="n">
+      <c r="E22" s="32"/>
+      <c r="F22" s="31" t="n">
         <f aca="false">(A22-1)*NBOXES+LBOX3</f>
         <v>31</v>
       </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="35" t="n">
+      <c r="G22" s="32"/>
+      <c r="H22" s="31" t="n">
         <f aca="false">(A22-1)*NBOXES+LBOX4</f>
         <v>32</v>
       </c>
-      <c r="I22" s="37"/>
+      <c r="I22" s="32"/>
       <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34" t="n">
+      <c r="A23" s="30" t="n">
         <v>9</v>
       </c>
-      <c r="B23" s="35" t="n">
+      <c r="B23" s="31" t="n">
         <f aca="false">(A23-1)*NBOXES+LBOX1</f>
         <v>33</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="35" t="n">
+      <c r="C23" s="32"/>
+      <c r="D23" s="31" t="n">
         <f aca="false">(A23-1)*NBOXES+LBOX2</f>
         <v>34</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="35" t="n">
+      <c r="E23" s="32"/>
+      <c r="F23" s="31" t="n">
         <f aca="false">(A23-1)*NBOXES+LBOX3</f>
         <v>35</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="35" t="n">
+      <c r="G23" s="32"/>
+      <c r="H23" s="31" t="n">
         <f aca="false">(A23-1)*NBOXES+LBOX4</f>
         <v>36</v>
       </c>
-      <c r="I23" s="37"/>
+      <c r="I23" s="32"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
       <c r="O23" s="0"/>
@@ -1621,1822 +1381,1822 @@
       <c r="S23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34" t="n">
+      <c r="A24" s="30" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="35" t="n">
+      <c r="B24" s="31" t="n">
         <f aca="false">(A24-1)*NBOXES+LBOX1</f>
         <v>37</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="35" t="n">
+      <c r="C24" s="32"/>
+      <c r="D24" s="31" t="n">
         <f aca="false">(A24-1)*NBOXES+LBOX2</f>
         <v>38</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="35" t="n">
+      <c r="E24" s="32"/>
+      <c r="F24" s="31" t="n">
         <f aca="false">(A24-1)*NBOXES+LBOX3</f>
         <v>39</v>
       </c>
-      <c r="G24" s="36"/>
-      <c r="H24" s="35" t="n">
+      <c r="G24" s="32"/>
+      <c r="H24" s="31" t="n">
         <f aca="false">(A24-1)*NBOXES+LBOX4</f>
         <v>40</v>
       </c>
-      <c r="I24" s="37"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="34" t="n">
+      <c r="A25" s="30" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="35" t="n">
+      <c r="B25" s="31" t="n">
         <f aca="false">(A25-1)*NBOXES+LBOX1</f>
         <v>41</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="35" t="n">
+      <c r="C25" s="32"/>
+      <c r="D25" s="31" t="n">
         <f aca="false">(A25-1)*NBOXES+LBOX2</f>
         <v>42</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="35" t="n">
+      <c r="E25" s="32"/>
+      <c r="F25" s="31" t="n">
         <f aca="false">(A25-1)*NBOXES+LBOX3</f>
         <v>43</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="35" t="n">
+      <c r="G25" s="32"/>
+      <c r="H25" s="31" t="n">
         <f aca="false">(A25-1)*NBOXES+LBOX4</f>
         <v>44</v>
       </c>
-      <c r="I25" s="37"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38" t="n">
+      <c r="A26" s="33" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="39" t="n">
+      <c r="B26" s="34" t="n">
         <f aca="false">(A26-1)*NBOXES+LBOX1</f>
         <v>45</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="39" t="n">
+      <c r="C26" s="35"/>
+      <c r="D26" s="34" t="n">
         <f aca="false">(A26-1)*NBOXES+LBOX2</f>
         <v>46</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="39" t="n">
+      <c r="E26" s="35"/>
+      <c r="F26" s="34" t="n">
         <f aca="false">(A26-1)*NBOXES+LBOX3</f>
         <v>47</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41" t="n">
+      <c r="G26" s="35"/>
+      <c r="H26" s="36" t="n">
         <f aca="false">(A26-1)*NBOXES+LBOX4</f>
         <v>48</v>
       </c>
-      <c r="I26" s="42"/>
+      <c r="I26" s="37"/>
       <c r="K26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H27" s="43" t="s">
+      <c r="H27" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="44" t="n">
+      <c r="I27" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C15:I26)-LEN(SUBSTITUTE(UPPER(C15:I26),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="27"/>
+      <c r="C28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="I29" s="26" t="s">
         <v>17</v>
       </c>
       <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30" t="n">
+      <c r="A30" s="27" t="n">
         <v>13</v>
       </c>
-      <c r="B30" s="31" t="n">
+      <c r="B30" s="28" t="n">
         <f aca="false">(A30-1)*NBOXES+LBOX1</f>
         <v>49</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31" t="n">
+      <c r="C30" s="29"/>
+      <c r="D30" s="28" t="n">
         <f aca="false">(A30-1)*NBOXES+LBOX2</f>
         <v>50</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="31" t="n">
+      <c r="E30" s="29"/>
+      <c r="F30" s="28" t="n">
         <f aca="false">(A30-1)*NBOXES+LBOX3</f>
         <v>51</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="31" t="n">
+      <c r="G30" s="29"/>
+      <c r="H30" s="28" t="n">
         <f aca="false">(A30-1)*NBOXES+LBOX4</f>
         <v>52</v>
       </c>
-      <c r="I30" s="33"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="34" t="n">
+      <c r="A31" s="30" t="n">
         <v>14</v>
       </c>
-      <c r="B31" s="35" t="n">
+      <c r="B31" s="31" t="n">
         <f aca="false">(A31-1)*NBOXES+LBOX1</f>
         <v>53</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="35" t="n">
+      <c r="C31" s="32"/>
+      <c r="D31" s="31" t="n">
         <f aca="false">(A31-1)*NBOXES+LBOX2</f>
         <v>54</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="35" t="n">
+      <c r="E31" s="32"/>
+      <c r="F31" s="31" t="n">
         <f aca="false">(A31-1)*NBOXES+LBOX3</f>
         <v>55</v>
       </c>
-      <c r="G31" s="36"/>
-      <c r="H31" s="35" t="n">
+      <c r="G31" s="32"/>
+      <c r="H31" s="31" t="n">
         <f aca="false">(A31-1)*NBOXES+LBOX4</f>
         <v>56</v>
       </c>
-      <c r="I31" s="37"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="34" t="n">
+      <c r="A32" s="30" t="n">
         <v>15</v>
       </c>
-      <c r="B32" s="35" t="n">
+      <c r="B32" s="31" t="n">
         <f aca="false">(A32-1)*NBOXES+LBOX1</f>
         <v>57</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="35" t="n">
+      <c r="C32" s="32"/>
+      <c r="D32" s="31" t="n">
         <f aca="false">(A32-1)*NBOXES+LBOX2</f>
         <v>58</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="35" t="n">
+      <c r="E32" s="32"/>
+      <c r="F32" s="31" t="n">
         <f aca="false">(A32-1)*NBOXES+LBOX3</f>
         <v>59</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="35" t="n">
+      <c r="G32" s="32"/>
+      <c r="H32" s="31" t="n">
         <f aca="false">(A32-1)*NBOXES+LBOX4</f>
         <v>60</v>
       </c>
-      <c r="I32" s="37"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="34" t="n">
+      <c r="A33" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="B33" s="35" t="n">
+      <c r="B33" s="31" t="n">
         <f aca="false">(A33-1)*NBOXES+LBOX1</f>
         <v>61</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="35" t="n">
+      <c r="C33" s="32"/>
+      <c r="D33" s="31" t="n">
         <f aca="false">(A33-1)*NBOXES+LBOX2</f>
         <v>62</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="35" t="n">
+      <c r="E33" s="32"/>
+      <c r="F33" s="31" t="n">
         <f aca="false">(A33-1)*NBOXES+LBOX3</f>
         <v>63</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="35" t="n">
+      <c r="G33" s="32"/>
+      <c r="H33" s="31" t="n">
         <f aca="false">(A33-1)*NBOXES+LBOX4</f>
         <v>64</v>
       </c>
-      <c r="I33" s="37"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="34" t="n">
+      <c r="A34" s="30" t="n">
         <v>17</v>
       </c>
-      <c r="B34" s="35" t="n">
+      <c r="B34" s="31" t="n">
         <f aca="false">(A34-1)*NBOXES+LBOX1</f>
         <v>65</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="35" t="n">
+      <c r="C34" s="32"/>
+      <c r="D34" s="31" t="n">
         <f aca="false">(A34-1)*NBOXES+LBOX2</f>
         <v>66</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="35" t="n">
+      <c r="E34" s="32"/>
+      <c r="F34" s="31" t="n">
         <f aca="false">(A34-1)*NBOXES+LBOX3</f>
         <v>67</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="35" t="n">
+      <c r="G34" s="32"/>
+      <c r="H34" s="31" t="n">
         <f aca="false">(A34-1)*NBOXES+LBOX4</f>
         <v>68</v>
       </c>
-      <c r="I34" s="37"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="34" t="n">
+      <c r="A35" s="30" t="n">
         <v>18</v>
       </c>
-      <c r="B35" s="35" t="n">
+      <c r="B35" s="31" t="n">
         <f aca="false">(A35-1)*NBOXES+LBOX1</f>
         <v>69</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="35" t="n">
+      <c r="C35" s="32"/>
+      <c r="D35" s="31" t="n">
         <f aca="false">(A35-1)*NBOXES+LBOX2</f>
         <v>70</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="35" t="n">
+      <c r="E35" s="32"/>
+      <c r="F35" s="31" t="n">
         <f aca="false">(A35-1)*NBOXES+LBOX3</f>
         <v>71</v>
       </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="35" t="n">
+      <c r="G35" s="32"/>
+      <c r="H35" s="31" t="n">
         <f aca="false">(A35-1)*NBOXES+LBOX4</f>
         <v>72</v>
       </c>
-      <c r="I35" s="37"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="34" t="n">
+      <c r="A36" s="30" t="n">
         <v>19</v>
       </c>
-      <c r="B36" s="35" t="n">
+      <c r="B36" s="31" t="n">
         <f aca="false">(A36-1)*NBOXES+LBOX1</f>
         <v>73</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="35" t="n">
+      <c r="C36" s="32"/>
+      <c r="D36" s="31" t="n">
         <f aca="false">(A36-1)*NBOXES+LBOX2</f>
         <v>74</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="35" t="n">
+      <c r="E36" s="32"/>
+      <c r="F36" s="31" t="n">
         <f aca="false">(A36-1)*NBOXES+LBOX3</f>
         <v>75</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="35" t="n">
+      <c r="G36" s="32"/>
+      <c r="H36" s="31" t="n">
         <f aca="false">(A36-1)*NBOXES+LBOX4</f>
         <v>76</v>
       </c>
-      <c r="I36" s="37"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="34" t="n">
+      <c r="A37" s="30" t="n">
         <v>20</v>
       </c>
-      <c r="B37" s="35" t="n">
+      <c r="B37" s="31" t="n">
         <f aca="false">(A37-1)*NBOXES+LBOX1</f>
         <v>77</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="35" t="n">
+      <c r="C37" s="32"/>
+      <c r="D37" s="31" t="n">
         <f aca="false">(A37-1)*NBOXES+LBOX2</f>
         <v>78</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="35" t="n">
+      <c r="E37" s="32"/>
+      <c r="F37" s="31" t="n">
         <f aca="false">(A37-1)*NBOXES+LBOX3</f>
         <v>79</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="35" t="n">
+      <c r="G37" s="32"/>
+      <c r="H37" s="31" t="n">
         <f aca="false">(A37-1)*NBOXES+LBOX4</f>
         <v>80</v>
       </c>
-      <c r="I37" s="37"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="34" t="n">
+      <c r="A38" s="30" t="n">
         <v>21</v>
       </c>
-      <c r="B38" s="35" t="n">
+      <c r="B38" s="31" t="n">
         <f aca="false">(A38-1)*NBOXES+LBOX1</f>
         <v>81</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="35" t="n">
+      <c r="C38" s="32"/>
+      <c r="D38" s="31" t="n">
         <f aca="false">(A38-1)*NBOXES+LBOX2</f>
         <v>82</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="35" t="n">
+      <c r="E38" s="32"/>
+      <c r="F38" s="31" t="n">
         <f aca="false">(A38-1)*NBOXES+LBOX3</f>
         <v>83</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="35" t="n">
+      <c r="G38" s="32"/>
+      <c r="H38" s="31" t="n">
         <f aca="false">(A38-1)*NBOXES+LBOX4</f>
         <v>84</v>
       </c>
-      <c r="I38" s="37"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="34" t="n">
+      <c r="A39" s="30" t="n">
         <v>22</v>
       </c>
-      <c r="B39" s="35" t="n">
+      <c r="B39" s="31" t="n">
         <f aca="false">(A39-1)*NBOXES+LBOX1</f>
         <v>85</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="35" t="n">
+      <c r="C39" s="32"/>
+      <c r="D39" s="31" t="n">
         <f aca="false">(A39-1)*NBOXES+LBOX2</f>
         <v>86</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="35" t="n">
+      <c r="E39" s="32"/>
+      <c r="F39" s="31" t="n">
         <f aca="false">(A39-1)*NBOXES+LBOX3</f>
         <v>87</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="35" t="n">
+      <c r="G39" s="32"/>
+      <c r="H39" s="31" t="n">
         <f aca="false">(A39-1)*NBOXES+LBOX4</f>
         <v>88</v>
       </c>
-      <c r="I39" s="37"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="34" t="n">
+      <c r="A40" s="30" t="n">
         <v>23</v>
       </c>
-      <c r="B40" s="35" t="n">
+      <c r="B40" s="31" t="n">
         <f aca="false">(A40-1)*NBOXES+LBOX1</f>
         <v>89</v>
       </c>
-      <c r="C40" s="37"/>
-      <c r="D40" s="35" t="n">
+      <c r="C40" s="32"/>
+      <c r="D40" s="31" t="n">
         <f aca="false">(A40-1)*NBOXES+LBOX2</f>
         <v>90</v>
       </c>
-      <c r="E40" s="37"/>
-      <c r="F40" s="35" t="n">
+      <c r="E40" s="32"/>
+      <c r="F40" s="31" t="n">
         <f aca="false">(A40-1)*NBOXES+LBOX3</f>
         <v>91</v>
       </c>
-      <c r="G40" s="37"/>
-      <c r="H40" s="35" t="n">
+      <c r="G40" s="32"/>
+      <c r="H40" s="31" t="n">
         <f aca="false">(A40-1)*NBOXES+LBOX4</f>
         <v>92</v>
       </c>
-      <c r="I40" s="37"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="38" t="n">
+      <c r="A41" s="33" t="n">
         <v>24</v>
       </c>
-      <c r="B41" s="39" t="n">
+      <c r="B41" s="34" t="n">
         <f aca="false">(A41-1)*NBOXES+LBOX1</f>
         <v>93</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="39" t="n">
+      <c r="C41" s="35"/>
+      <c r="D41" s="34" t="n">
         <f aca="false">(A41-1)*NBOXES+LBOX2</f>
         <v>94</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="39" t="n">
+      <c r="E41" s="35"/>
+      <c r="F41" s="34" t="n">
         <f aca="false">(A41-1)*NBOXES+LBOX3</f>
         <v>95</v>
       </c>
-      <c r="G41" s="40"/>
-      <c r="H41" s="39" t="n">
+      <c r="G41" s="35"/>
+      <c r="H41" s="34" t="n">
         <f aca="false">(A41-1)*NBOXES+LBOX4</f>
         <v>96</v>
       </c>
-      <c r="I41" s="45"/>
+      <c r="I41" s="35"/>
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="44" t="n">
+      <c r="I42" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C30:I41)-LEN(SUBSTITUTE(UPPER(C30:I41),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="27"/>
+      <c r="C43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="28" t="s">
+      <c r="H44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="29" t="s">
+      <c r="I44" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="30" t="n">
+      <c r="A45" s="27" t="n">
         <v>25</v>
       </c>
-      <c r="B45" s="31" t="n">
+      <c r="B45" s="28" t="n">
         <f aca="false">(A45-1)*NBOXES+LBOX1</f>
         <v>97</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="31" t="n">
+      <c r="C45" s="29"/>
+      <c r="D45" s="28" t="n">
         <f aca="false">(A45-1)*NBOXES+LBOX2</f>
         <v>98</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="31" t="n">
+      <c r="E45" s="29"/>
+      <c r="F45" s="28" t="n">
         <f aca="false">(A45-1)*NBOXES+LBOX3</f>
         <v>99</v>
       </c>
-      <c r="G45" s="32"/>
-      <c r="H45" s="31" t="n">
+      <c r="G45" s="29"/>
+      <c r="H45" s="28" t="n">
         <f aca="false">(A45-1)*NBOXES+LBOX4</f>
         <v>100</v>
       </c>
-      <c r="I45" s="33"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="34" t="n">
+      <c r="A46" s="30" t="n">
         <v>26</v>
       </c>
-      <c r="B46" s="35" t="n">
+      <c r="B46" s="31" t="n">
         <f aca="false">(A46-1)*NBOXES+LBOX1</f>
         <v>101</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="35" t="n">
+      <c r="C46" s="32"/>
+      <c r="D46" s="31" t="n">
         <f aca="false">(A46-1)*NBOXES+LBOX2</f>
         <v>102</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="35" t="n">
+      <c r="E46" s="32"/>
+      <c r="F46" s="31" t="n">
         <f aca="false">(A46-1)*NBOXES+LBOX3</f>
         <v>103</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="H46" s="35" t="n">
+      <c r="G46" s="32"/>
+      <c r="H46" s="31" t="n">
         <f aca="false">(A46-1)*NBOXES+LBOX4</f>
         <v>104</v>
       </c>
-      <c r="I46" s="37"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="34" t="n">
+      <c r="A47" s="30" t="n">
         <v>27</v>
       </c>
-      <c r="B47" s="35" t="n">
+      <c r="B47" s="31" t="n">
         <f aca="false">(A47-1)*NBOXES+LBOX1</f>
         <v>105</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="35" t="n">
+      <c r="C47" s="32"/>
+      <c r="D47" s="31" t="n">
         <f aca="false">(A47-1)*NBOXES+LBOX2</f>
         <v>106</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="35" t="n">
+      <c r="E47" s="32"/>
+      <c r="F47" s="31" t="n">
         <f aca="false">(A47-1)*NBOXES+LBOX3</f>
         <v>107</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="H47" s="35" t="n">
+      <c r="G47" s="32"/>
+      <c r="H47" s="31" t="n">
         <f aca="false">(A47-1)*NBOXES+LBOX4</f>
         <v>108</v>
       </c>
-      <c r="I47" s="37"/>
+      <c r="I47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="34" t="n">
+      <c r="A48" s="30" t="n">
         <v>28</v>
       </c>
-      <c r="B48" s="35" t="n">
+      <c r="B48" s="31" t="n">
         <f aca="false">(A48-1)*NBOXES+LBOX1</f>
         <v>109</v>
       </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="35" t="n">
+      <c r="C48" s="32"/>
+      <c r="D48" s="31" t="n">
         <f aca="false">(A48-1)*NBOXES+LBOX2</f>
         <v>110</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="35" t="n">
+      <c r="E48" s="32"/>
+      <c r="F48" s="31" t="n">
         <f aca="false">(A48-1)*NBOXES+LBOX3</f>
         <v>111</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="35" t="n">
+      <c r="G48" s="32"/>
+      <c r="H48" s="31" t="n">
         <f aca="false">(A48-1)*NBOXES+LBOX4</f>
         <v>112</v>
       </c>
-      <c r="I48" s="37"/>
+      <c r="I48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="34" t="n">
+      <c r="A49" s="30" t="n">
         <v>29</v>
       </c>
-      <c r="B49" s="35" t="n">
+      <c r="B49" s="31" t="n">
         <f aca="false">(A49-1)*NBOXES+LBOX1</f>
         <v>113</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="35" t="n">
+      <c r="C49" s="32"/>
+      <c r="D49" s="31" t="n">
         <f aca="false">(A49-1)*NBOXES+LBOX2</f>
         <v>114</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="35" t="n">
+      <c r="E49" s="32"/>
+      <c r="F49" s="31" t="n">
         <f aca="false">(A49-1)*NBOXES+LBOX3</f>
         <v>115</v>
       </c>
-      <c r="G49" s="36"/>
-      <c r="H49" s="35" t="n">
+      <c r="G49" s="32"/>
+      <c r="H49" s="31" t="n">
         <f aca="false">(A49-1)*NBOXES+LBOX4</f>
         <v>116</v>
       </c>
-      <c r="I49" s="37"/>
+      <c r="I49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="34" t="n">
+      <c r="A50" s="30" t="n">
         <v>30</v>
       </c>
-      <c r="B50" s="35" t="n">
+      <c r="B50" s="31" t="n">
         <f aca="false">(A50-1)*NBOXES+LBOX1</f>
         <v>117</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="35" t="n">
+      <c r="C50" s="32"/>
+      <c r="D50" s="31" t="n">
         <f aca="false">(A50-1)*NBOXES+LBOX2</f>
         <v>118</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="35" t="n">
+      <c r="E50" s="32"/>
+      <c r="F50" s="31" t="n">
         <f aca="false">(A50-1)*NBOXES+LBOX3</f>
         <v>119</v>
       </c>
-      <c r="G50" s="36"/>
-      <c r="H50" s="35" t="n">
+      <c r="G50" s="32"/>
+      <c r="H50" s="31" t="n">
         <f aca="false">(A50-1)*NBOXES+LBOX4</f>
         <v>120</v>
       </c>
-      <c r="I50" s="37"/>
+      <c r="I50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="34" t="n">
+      <c r="A51" s="30" t="n">
         <v>31</v>
       </c>
-      <c r="B51" s="35" t="n">
+      <c r="B51" s="31" t="n">
         <f aca="false">(A51-1)*NBOXES+LBOX1</f>
         <v>121</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="35" t="n">
+      <c r="C51" s="32"/>
+      <c r="D51" s="31" t="n">
         <f aca="false">(A51-1)*NBOXES+LBOX2</f>
         <v>122</v>
       </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="35" t="n">
+      <c r="E51" s="32"/>
+      <c r="F51" s="31" t="n">
         <f aca="false">(A51-1)*NBOXES+LBOX3</f>
         <v>123</v>
       </c>
-      <c r="G51" s="36"/>
-      <c r="H51" s="35" t="n">
+      <c r="G51" s="32"/>
+      <c r="H51" s="31" t="n">
         <f aca="false">(A51-1)*NBOXES+LBOX4</f>
         <v>124</v>
       </c>
-      <c r="I51" s="37"/>
+      <c r="I51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="34" t="n">
+      <c r="A52" s="30" t="n">
         <v>32</v>
       </c>
-      <c r="B52" s="35" t="n">
+      <c r="B52" s="31" t="n">
         <f aca="false">(A52-1)*NBOXES+LBOX1</f>
         <v>125</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="35" t="n">
+      <c r="C52" s="32"/>
+      <c r="D52" s="31" t="n">
         <f aca="false">(A52-1)*NBOXES+LBOX2</f>
         <v>126</v>
       </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="35" t="n">
+      <c r="E52" s="32"/>
+      <c r="F52" s="31" t="n">
         <f aca="false">(A52-1)*NBOXES+LBOX3</f>
         <v>127</v>
       </c>
-      <c r="G52" s="36"/>
-      <c r="H52" s="35" t="n">
+      <c r="G52" s="32"/>
+      <c r="H52" s="31" t="n">
         <f aca="false">(A52-1)*NBOXES+LBOX4</f>
         <v>128</v>
       </c>
-      <c r="I52" s="37"/>
+      <c r="I52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="34" t="n">
+      <c r="A53" s="30" t="n">
         <v>33</v>
       </c>
-      <c r="B53" s="35" t="n">
+      <c r="B53" s="31" t="n">
         <f aca="false">(A53-1)*NBOXES+LBOX1</f>
         <v>129</v>
       </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="35" t="n">
+      <c r="C53" s="32"/>
+      <c r="D53" s="31" t="n">
         <f aca="false">(A53-1)*NBOXES+LBOX2</f>
         <v>130</v>
       </c>
-      <c r="E53" s="36"/>
-      <c r="F53" s="35" t="n">
+      <c r="E53" s="32"/>
+      <c r="F53" s="31" t="n">
         <f aca="false">(A53-1)*NBOXES+LBOX3</f>
         <v>131</v>
       </c>
-      <c r="G53" s="36"/>
-      <c r="H53" s="35" t="n">
+      <c r="G53" s="32"/>
+      <c r="H53" s="31" t="n">
         <f aca="false">(A53-1)*NBOXES+LBOX4</f>
         <v>132</v>
       </c>
-      <c r="I53" s="37"/>
+      <c r="I53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="34" t="n">
+      <c r="A54" s="30" t="n">
         <v>34</v>
       </c>
-      <c r="B54" s="35" t="n">
+      <c r="B54" s="31" t="n">
         <f aca="false">(A54-1)*NBOXES+LBOX1</f>
         <v>133</v>
       </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="35" t="n">
+      <c r="C54" s="32"/>
+      <c r="D54" s="31" t="n">
         <f aca="false">(A54-1)*NBOXES+LBOX2</f>
         <v>134</v>
       </c>
-      <c r="E54" s="36"/>
-      <c r="F54" s="35" t="n">
+      <c r="E54" s="32"/>
+      <c r="F54" s="31" t="n">
         <f aca="false">(A54-1)*NBOXES+LBOX3</f>
         <v>135</v>
       </c>
-      <c r="G54" s="36"/>
-      <c r="H54" s="35" t="n">
+      <c r="G54" s="32"/>
+      <c r="H54" s="31" t="n">
         <f aca="false">(A54-1)*NBOXES+LBOX4</f>
         <v>136</v>
       </c>
-      <c r="I54" s="37"/>
+      <c r="I54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="34" t="n">
+      <c r="A55" s="30" t="n">
         <v>35</v>
       </c>
-      <c r="B55" s="35" t="n">
+      <c r="B55" s="31" t="n">
         <f aca="false">(A55-1)*NBOXES+LBOX1</f>
         <v>137</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="35" t="n">
+      <c r="C55" s="32"/>
+      <c r="D55" s="31" t="n">
         <f aca="false">(A55-1)*NBOXES+LBOX2</f>
         <v>138</v>
       </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="35" t="n">
+      <c r="E55" s="32"/>
+      <c r="F55" s="31" t="n">
         <f aca="false">(A55-1)*NBOXES+LBOX3</f>
         <v>139</v>
       </c>
-      <c r="G55" s="37"/>
-      <c r="H55" s="35" t="n">
+      <c r="G55" s="32"/>
+      <c r="H55" s="31" t="n">
         <f aca="false">(A55-1)*NBOXES+LBOX4</f>
         <v>140</v>
       </c>
-      <c r="I55" s="37"/>
+      <c r="I55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="38" t="n">
+      <c r="A56" s="33" t="n">
         <v>36</v>
       </c>
-      <c r="B56" s="39" t="n">
+      <c r="B56" s="34" t="n">
         <f aca="false">(A56-1)*NBOXES+LBOX1</f>
         <v>141</v>
       </c>
-      <c r="C56" s="40"/>
-      <c r="D56" s="39" t="n">
+      <c r="C56" s="35"/>
+      <c r="D56" s="34" t="n">
         <f aca="false">(A56-1)*NBOXES+LBOX2</f>
         <v>142</v>
       </c>
-      <c r="E56" s="40"/>
-      <c r="F56" s="39" t="n">
+      <c r="E56" s="35"/>
+      <c r="F56" s="34" t="n">
         <f aca="false">(A56-1)*NBOXES+LBOX3</f>
         <v>143</v>
       </c>
-      <c r="G56" s="40"/>
-      <c r="H56" s="39" t="n">
+      <c r="G56" s="35"/>
+      <c r="H56" s="34" t="n">
         <f aca="false">(A56-1)*NBOXES+LBOX4</f>
         <v>144</v>
       </c>
-      <c r="I56" s="45"/>
+      <c r="I56" s="35"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="43" t="s">
+      <c r="H57" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I57" s="44" t="n">
+      <c r="I57" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C45:I56)-LEN(SUBSTITUTE(UPPER(C45:I56),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="27"/>
+      <c r="C62" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E63" s="29" t="s">
+      <c r="E63" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F63" s="28" t="s">
+      <c r="F63" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="29" t="s">
+      <c r="G63" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H63" s="28" t="s">
+      <c r="H63" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I63" s="29" t="s">
+      <c r="I63" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="46" t="n">
+      <c r="A64" s="40" t="n">
         <v>37</v>
       </c>
-      <c r="B64" s="31" t="n">
+      <c r="B64" s="28" t="n">
         <f aca="false">(A64-1)*NBOXES+LBOX1</f>
         <v>145</v>
       </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="31" t="n">
+      <c r="C64" s="29"/>
+      <c r="D64" s="28" t="n">
         <f aca="false">(A64-1)*NBOXES+LBOX2</f>
         <v>146</v>
       </c>
-      <c r="E64" s="32"/>
-      <c r="F64" s="31" t="n">
+      <c r="E64" s="29"/>
+      <c r="F64" s="28" t="n">
         <f aca="false">(A64-1)*NBOXES+LBOX3</f>
         <v>147</v>
       </c>
-      <c r="G64" s="32"/>
-      <c r="H64" s="31" t="n">
+      <c r="G64" s="29"/>
+      <c r="H64" s="28" t="n">
         <f aca="false">(A64-1)*NBOXES+LBOX4</f>
         <v>148</v>
       </c>
-      <c r="I64" s="33"/>
+      <c r="I64" s="29"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="34" t="n">
+      <c r="A65" s="30" t="n">
         <v>38</v>
       </c>
-      <c r="B65" s="35" t="n">
+      <c r="B65" s="31" t="n">
         <f aca="false">(A65-1)*NBOXES+LBOX1</f>
         <v>149</v>
       </c>
-      <c r="C65" s="36"/>
-      <c r="D65" s="35" t="n">
+      <c r="C65" s="32"/>
+      <c r="D65" s="31" t="n">
         <f aca="false">(A65-1)*NBOXES+LBOX2</f>
         <v>150</v>
       </c>
-      <c r="E65" s="36"/>
-      <c r="F65" s="35" t="n">
+      <c r="E65" s="32"/>
+      <c r="F65" s="31" t="n">
         <f aca="false">(A65-1)*NBOXES+LBOX3</f>
         <v>151</v>
       </c>
-      <c r="G65" s="36"/>
-      <c r="H65" s="35" t="n">
+      <c r="G65" s="32"/>
+      <c r="H65" s="31" t="n">
         <f aca="false">(A65-1)*NBOXES+LBOX4</f>
         <v>152</v>
       </c>
-      <c r="I65" s="37"/>
+      <c r="I65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="30" t="n">
+      <c r="A66" s="27" t="n">
         <v>39</v>
       </c>
-      <c r="B66" s="35" t="n">
+      <c r="B66" s="31" t="n">
         <f aca="false">(A66-1)*NBOXES+LBOX1</f>
         <v>153</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="35" t="n">
+      <c r="C66" s="32"/>
+      <c r="D66" s="31" t="n">
         <f aca="false">(A66-1)*NBOXES+LBOX2</f>
         <v>154</v>
       </c>
-      <c r="E66" s="36"/>
-      <c r="F66" s="35" t="n">
+      <c r="E66" s="32"/>
+      <c r="F66" s="31" t="n">
         <f aca="false">(A66-1)*NBOXES+LBOX3</f>
         <v>155</v>
       </c>
-      <c r="G66" s="36"/>
-      <c r="H66" s="35" t="n">
+      <c r="G66" s="32"/>
+      <c r="H66" s="31" t="n">
         <f aca="false">(A66-1)*NBOXES+LBOX4</f>
         <v>156</v>
       </c>
-      <c r="I66" s="37"/>
+      <c r="I66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="34" t="n">
+      <c r="A67" s="30" t="n">
         <v>40</v>
       </c>
-      <c r="B67" s="35" t="n">
+      <c r="B67" s="31" t="n">
         <f aca="false">(A67-1)*NBOXES+LBOX1</f>
         <v>157</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="35" t="n">
+      <c r="C67" s="32"/>
+      <c r="D67" s="31" t="n">
         <f aca="false">(A67-1)*NBOXES+LBOX2</f>
         <v>158</v>
       </c>
-      <c r="E67" s="36"/>
-      <c r="F67" s="35" t="n">
+      <c r="E67" s="32"/>
+      <c r="F67" s="31" t="n">
         <f aca="false">(A67-1)*NBOXES+LBOX3</f>
         <v>159</v>
       </c>
-      <c r="G67" s="36"/>
-      <c r="H67" s="35" t="n">
+      <c r="G67" s="32"/>
+      <c r="H67" s="31" t="n">
         <f aca="false">(A67-1)*NBOXES+LBOX4</f>
         <v>160</v>
       </c>
-      <c r="I67" s="37"/>
+      <c r="I67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="30" t="n">
+      <c r="A68" s="27" t="n">
         <v>41</v>
       </c>
-      <c r="B68" s="35" t="n">
+      <c r="B68" s="31" t="n">
         <f aca="false">(A68-1)*NBOXES+LBOX1</f>
         <v>161</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="35" t="n">
+      <c r="C68" s="32"/>
+      <c r="D68" s="31" t="n">
         <f aca="false">(A68-1)*NBOXES+LBOX2</f>
         <v>162</v>
       </c>
-      <c r="E68" s="36"/>
-      <c r="F68" s="35" t="n">
+      <c r="E68" s="32"/>
+      <c r="F68" s="31" t="n">
         <f aca="false">(A68-1)*NBOXES+LBOX3</f>
         <v>163</v>
       </c>
-      <c r="G68" s="36"/>
-      <c r="H68" s="35" t="n">
+      <c r="G68" s="32"/>
+      <c r="H68" s="31" t="n">
         <f aca="false">(A68-1)*NBOXES+LBOX4</f>
         <v>164</v>
       </c>
-      <c r="I68" s="37"/>
+      <c r="I68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="34" t="n">
+      <c r="A69" s="30" t="n">
         <v>42</v>
       </c>
-      <c r="B69" s="35" t="n">
+      <c r="B69" s="31" t="n">
         <f aca="false">(A69-1)*NBOXES+LBOX1</f>
         <v>165</v>
       </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="35" t="n">
+      <c r="C69" s="32"/>
+      <c r="D69" s="31" t="n">
         <f aca="false">(A69-1)*NBOXES+LBOX2</f>
         <v>166</v>
       </c>
-      <c r="E69" s="36"/>
-      <c r="F69" s="35" t="n">
+      <c r="E69" s="32"/>
+      <c r="F69" s="31" t="n">
         <f aca="false">(A69-1)*NBOXES+LBOX3</f>
         <v>167</v>
       </c>
-      <c r="G69" s="36"/>
-      <c r="H69" s="35" t="n">
+      <c r="G69" s="32"/>
+      <c r="H69" s="31" t="n">
         <f aca="false">(A69-1)*NBOXES+LBOX4</f>
         <v>168</v>
       </c>
-      <c r="I69" s="37"/>
+      <c r="I69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="30" t="n">
+      <c r="A70" s="27" t="n">
         <v>43</v>
       </c>
-      <c r="B70" s="35" t="n">
+      <c r="B70" s="31" t="n">
         <f aca="false">(A70-1)*NBOXES+LBOX1</f>
         <v>169</v>
       </c>
-      <c r="C70" s="36"/>
-      <c r="D70" s="35" t="n">
+      <c r="C70" s="32"/>
+      <c r="D70" s="31" t="n">
         <f aca="false">(A70-1)*NBOXES+LBOX2</f>
         <v>170</v>
       </c>
-      <c r="E70" s="36"/>
-      <c r="F70" s="35" t="n">
+      <c r="E70" s="32"/>
+      <c r="F70" s="31" t="n">
         <f aca="false">(A70-1)*NBOXES+LBOX3</f>
         <v>171</v>
       </c>
-      <c r="G70" s="36"/>
-      <c r="H70" s="35" t="n">
+      <c r="G70" s="32"/>
+      <c r="H70" s="31" t="n">
         <f aca="false">(A70-1)*NBOXES+LBOX4</f>
         <v>172</v>
       </c>
-      <c r="I70" s="37"/>
+      <c r="I70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="34" t="n">
+      <c r="A71" s="30" t="n">
         <v>44</v>
       </c>
-      <c r="B71" s="35" t="n">
+      <c r="B71" s="31" t="n">
         <f aca="false">(A71-1)*NBOXES+LBOX1</f>
         <v>173</v>
       </c>
-      <c r="C71" s="36"/>
-      <c r="D71" s="35" t="n">
+      <c r="C71" s="32"/>
+      <c r="D71" s="31" t="n">
         <f aca="false">(A71-1)*NBOXES+LBOX2</f>
         <v>174</v>
       </c>
-      <c r="E71" s="36"/>
-      <c r="F71" s="35" t="n">
+      <c r="E71" s="32"/>
+      <c r="F71" s="31" t="n">
         <f aca="false">(A71-1)*NBOXES+LBOX3</f>
         <v>175</v>
       </c>
-      <c r="G71" s="36"/>
-      <c r="H71" s="35" t="n">
+      <c r="G71" s="32"/>
+      <c r="H71" s="31" t="n">
         <f aca="false">(A71-1)*NBOXES+LBOX4</f>
         <v>176</v>
       </c>
-      <c r="I71" s="37"/>
+      <c r="I71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="30" t="n">
+      <c r="A72" s="27" t="n">
         <v>45</v>
       </c>
-      <c r="B72" s="35" t="n">
+      <c r="B72" s="31" t="n">
         <f aca="false">(A72-1)*NBOXES+LBOX1</f>
         <v>177</v>
       </c>
-      <c r="C72" s="36"/>
-      <c r="D72" s="35" t="n">
+      <c r="C72" s="32"/>
+      <c r="D72" s="31" t="n">
         <f aca="false">(A72-1)*NBOXES+LBOX2</f>
         <v>178</v>
       </c>
-      <c r="E72" s="36"/>
-      <c r="F72" s="35" t="n">
+      <c r="E72" s="32"/>
+      <c r="F72" s="31" t="n">
         <f aca="false">(A72-1)*NBOXES+LBOX3</f>
         <v>179</v>
       </c>
-      <c r="G72" s="36"/>
-      <c r="H72" s="35" t="n">
+      <c r="G72" s="32"/>
+      <c r="H72" s="31" t="n">
         <f aca="false">(A72-1)*NBOXES+LBOX4</f>
         <v>180</v>
       </c>
-      <c r="I72" s="37"/>
+      <c r="I72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="34" t="n">
+      <c r="A73" s="30" t="n">
         <v>46</v>
       </c>
-      <c r="B73" s="35" t="n">
+      <c r="B73" s="31" t="n">
         <f aca="false">(A73-1)*NBOXES+LBOX1</f>
         <v>181</v>
       </c>
-      <c r="C73" s="36"/>
-      <c r="D73" s="35" t="n">
+      <c r="C73" s="32"/>
+      <c r="D73" s="31" t="n">
         <f aca="false">(A73-1)*NBOXES+LBOX2</f>
         <v>182</v>
       </c>
-      <c r="E73" s="36"/>
-      <c r="F73" s="35" t="n">
+      <c r="E73" s="32"/>
+      <c r="F73" s="31" t="n">
         <f aca="false">(A73-1)*NBOXES+LBOX3</f>
         <v>183</v>
       </c>
-      <c r="G73" s="36"/>
-      <c r="H73" s="35" t="n">
+      <c r="G73" s="32"/>
+      <c r="H73" s="31" t="n">
         <f aca="false">(A73-1)*NBOXES+LBOX4</f>
         <v>184</v>
       </c>
-      <c r="I73" s="37"/>
+      <c r="I73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="30" t="n">
+      <c r="A74" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="B74" s="35" t="n">
+      <c r="B74" s="31" t="n">
         <f aca="false">(A74-1)*NBOXES+LBOX1</f>
         <v>185</v>
       </c>
-      <c r="C74" s="37"/>
-      <c r="D74" s="35" t="n">
+      <c r="C74" s="32"/>
+      <c r="D74" s="31" t="n">
         <f aca="false">(A74-1)*NBOXES+LBOX2</f>
         <v>186</v>
       </c>
-      <c r="E74" s="37"/>
-      <c r="F74" s="35" t="n">
+      <c r="E74" s="32"/>
+      <c r="F74" s="31" t="n">
         <f aca="false">(A74-1)*NBOXES+LBOX3</f>
         <v>187</v>
       </c>
-      <c r="G74" s="37"/>
-      <c r="H74" s="35" t="n">
+      <c r="G74" s="32"/>
+      <c r="H74" s="31" t="n">
         <f aca="false">(A74-1)*NBOXES+LBOX4</f>
         <v>188</v>
       </c>
-      <c r="I74" s="37"/>
+      <c r="I74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="38" t="n">
+      <c r="A75" s="33" t="n">
         <v>48</v>
       </c>
-      <c r="B75" s="39" t="n">
+      <c r="B75" s="34" t="n">
         <f aca="false">(A75-1)*NBOXES+LBOX1</f>
         <v>189</v>
       </c>
-      <c r="C75" s="40"/>
-      <c r="D75" s="39" t="n">
+      <c r="C75" s="35"/>
+      <c r="D75" s="34" t="n">
         <f aca="false">(A75-1)*NBOXES+LBOX2</f>
         <v>190</v>
       </c>
-      <c r="E75" s="40"/>
-      <c r="F75" s="39" t="n">
+      <c r="E75" s="35"/>
+      <c r="F75" s="34" t="n">
         <f aca="false">(A75-1)*NBOXES+LBOX3</f>
         <v>191</v>
       </c>
-      <c r="G75" s="40"/>
-      <c r="H75" s="39" t="n">
+      <c r="G75" s="35"/>
+      <c r="H75" s="34" t="n">
         <f aca="false">(A75-1)*NBOXES+LBOX4</f>
         <v>192</v>
       </c>
-      <c r="I75" s="45"/>
+      <c r="I75" s="35"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H76" s="43" t="s">
+      <c r="H76" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I76" s="44" t="n">
+      <c r="I76" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C64:I75)-LEN(SUBSTITUTE(UPPER(C64:I75),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="27"/>
+      <c r="C77" s="24"/>
     </row>
     <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="28" t="s">
+      <c r="D78" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="29" t="s">
+      <c r="E78" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F78" s="28" t="s">
+      <c r="F78" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G78" s="29" t="s">
+      <c r="G78" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H78" s="28" t="s">
+      <c r="H78" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I78" s="29" t="s">
+      <c r="I78" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="46" t="n">
+      <c r="A79" s="40" t="n">
         <v>49</v>
       </c>
-      <c r="B79" s="31" t="n">
+      <c r="B79" s="28" t="n">
         <f aca="false">(A79-1)*NBOXES+LBOX1</f>
         <v>193</v>
       </c>
-      <c r="C79" s="32"/>
-      <c r="D79" s="31" t="n">
+      <c r="C79" s="29"/>
+      <c r="D79" s="28" t="n">
         <f aca="false">(A79-1)*NBOXES+LBOX2</f>
         <v>194</v>
       </c>
-      <c r="E79" s="32"/>
-      <c r="F79" s="31" t="n">
+      <c r="E79" s="29"/>
+      <c r="F79" s="28" t="n">
         <f aca="false">(A79-1)*NBOXES+LBOX3</f>
         <v>195</v>
       </c>
-      <c r="G79" s="32"/>
-      <c r="H79" s="31" t="n">
+      <c r="G79" s="29"/>
+      <c r="H79" s="28" t="n">
         <f aca="false">(A79-1)*NBOXES+LBOX4</f>
         <v>196</v>
       </c>
-      <c r="I79" s="33"/>
+      <c r="I79" s="29"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="34" t="n">
+      <c r="A80" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="B80" s="35" t="n">
+      <c r="B80" s="31" t="n">
         <f aca="false">(A80-1)*NBOXES+LBOX1</f>
         <v>197</v>
       </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="35" t="n">
+      <c r="C80" s="32"/>
+      <c r="D80" s="31" t="n">
         <f aca="false">(A80-1)*NBOXES+LBOX2</f>
         <v>198</v>
       </c>
-      <c r="E80" s="36"/>
-      <c r="F80" s="35" t="n">
+      <c r="E80" s="32"/>
+      <c r="F80" s="31" t="n">
         <f aca="false">(A80-1)*NBOXES+LBOX3</f>
         <v>199</v>
       </c>
-      <c r="G80" s="36"/>
-      <c r="H80" s="35" t="n">
+      <c r="G80" s="32"/>
+      <c r="H80" s="31" t="n">
         <f aca="false">(A80-1)*NBOXES+LBOX4</f>
         <v>200</v>
       </c>
-      <c r="I80" s="37"/>
+      <c r="I80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="30" t="n">
+      <c r="A81" s="27" t="n">
         <v>51</v>
       </c>
-      <c r="B81" s="35" t="n">
+      <c r="B81" s="31" t="n">
         <f aca="false">(A81-1)*NBOXES+LBOX1</f>
         <v>201</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="35" t="n">
+      <c r="C81" s="32"/>
+      <c r="D81" s="31" t="n">
         <f aca="false">(A81-1)*NBOXES+LBOX2</f>
         <v>202</v>
       </c>
-      <c r="E81" s="36"/>
-      <c r="F81" s="35" t="n">
+      <c r="E81" s="32"/>
+      <c r="F81" s="31" t="n">
         <f aca="false">(A81-1)*NBOXES+LBOX3</f>
         <v>203</v>
       </c>
-      <c r="G81" s="36"/>
-      <c r="H81" s="35" t="n">
+      <c r="G81" s="32"/>
+      <c r="H81" s="31" t="n">
         <f aca="false">(A81-1)*NBOXES+LBOX4</f>
         <v>204</v>
       </c>
-      <c r="I81" s="37"/>
+      <c r="I81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="34" t="n">
+      <c r="A82" s="30" t="n">
         <v>52</v>
       </c>
-      <c r="B82" s="35" t="n">
+      <c r="B82" s="31" t="n">
         <f aca="false">(A82-1)*NBOXES+LBOX1</f>
         <v>205</v>
       </c>
-      <c r="C82" s="36"/>
-      <c r="D82" s="35" t="n">
+      <c r="C82" s="32"/>
+      <c r="D82" s="31" t="n">
         <f aca="false">(A82-1)*NBOXES+LBOX2</f>
         <v>206</v>
       </c>
-      <c r="E82" s="36"/>
-      <c r="F82" s="35" t="n">
+      <c r="E82" s="32"/>
+      <c r="F82" s="31" t="n">
         <f aca="false">(A82-1)*NBOXES+LBOX3</f>
         <v>207</v>
       </c>
-      <c r="G82" s="36"/>
-      <c r="H82" s="35" t="n">
+      <c r="G82" s="32"/>
+      <c r="H82" s="31" t="n">
         <f aca="false">(A82-1)*NBOXES+LBOX4</f>
         <v>208</v>
       </c>
-      <c r="I82" s="37"/>
+      <c r="I82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="30" t="n">
+      <c r="A83" s="27" t="n">
         <v>53</v>
       </c>
-      <c r="B83" s="35" t="n">
+      <c r="B83" s="31" t="n">
         <f aca="false">(A83-1)*NBOXES+LBOX1</f>
         <v>209</v>
       </c>
-      <c r="C83" s="36"/>
-      <c r="D83" s="35" t="n">
+      <c r="C83" s="32"/>
+      <c r="D83" s="31" t="n">
         <f aca="false">(A83-1)*NBOXES+LBOX2</f>
         <v>210</v>
       </c>
-      <c r="E83" s="36"/>
-      <c r="F83" s="35" t="n">
+      <c r="E83" s="32"/>
+      <c r="F83" s="31" t="n">
         <f aca="false">(A83-1)*NBOXES+LBOX3</f>
         <v>211</v>
       </c>
-      <c r="G83" s="36"/>
-      <c r="H83" s="35" t="n">
+      <c r="G83" s="32"/>
+      <c r="H83" s="31" t="n">
         <f aca="false">(A83-1)*NBOXES+LBOX4</f>
         <v>212</v>
       </c>
-      <c r="I83" s="37"/>
+      <c r="I83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="34" t="n">
+      <c r="A84" s="30" t="n">
         <v>54</v>
       </c>
-      <c r="B84" s="35" t="n">
+      <c r="B84" s="31" t="n">
         <f aca="false">(A84-1)*NBOXES+LBOX1</f>
         <v>213</v>
       </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="35" t="n">
+      <c r="C84" s="32"/>
+      <c r="D84" s="31" t="n">
         <f aca="false">(A84-1)*NBOXES+LBOX2</f>
         <v>214</v>
       </c>
-      <c r="E84" s="36"/>
-      <c r="F84" s="35" t="n">
+      <c r="E84" s="32"/>
+      <c r="F84" s="31" t="n">
         <f aca="false">(A84-1)*NBOXES+LBOX3</f>
         <v>215</v>
       </c>
-      <c r="G84" s="36"/>
-      <c r="H84" s="35" t="n">
+      <c r="G84" s="32"/>
+      <c r="H84" s="31" t="n">
         <f aca="false">(A84-1)*NBOXES+LBOX4</f>
         <v>216</v>
       </c>
-      <c r="I84" s="37"/>
+      <c r="I84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="30" t="n">
+      <c r="A85" s="27" t="n">
         <v>55</v>
       </c>
-      <c r="B85" s="35" t="n">
+      <c r="B85" s="31" t="n">
         <f aca="false">(A85-1)*NBOXES+LBOX1</f>
         <v>217</v>
       </c>
-      <c r="C85" s="36"/>
-      <c r="D85" s="35" t="n">
+      <c r="C85" s="32"/>
+      <c r="D85" s="31" t="n">
         <f aca="false">(A85-1)*NBOXES+LBOX2</f>
         <v>218</v>
       </c>
-      <c r="E85" s="36"/>
-      <c r="F85" s="35" t="n">
+      <c r="E85" s="32"/>
+      <c r="F85" s="31" t="n">
         <f aca="false">(A85-1)*NBOXES+LBOX3</f>
         <v>219</v>
       </c>
-      <c r="G85" s="36"/>
-      <c r="H85" s="35" t="n">
+      <c r="G85" s="32"/>
+      <c r="H85" s="31" t="n">
         <f aca="false">(A85-1)*NBOXES+LBOX4</f>
         <v>220</v>
       </c>
-      <c r="I85" s="37"/>
+      <c r="I85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="34" t="n">
+      <c r="A86" s="30" t="n">
         <v>56</v>
       </c>
-      <c r="B86" s="35" t="n">
+      <c r="B86" s="31" t="n">
         <f aca="false">(A86-1)*NBOXES+LBOX1</f>
         <v>221</v>
       </c>
-      <c r="C86" s="36"/>
-      <c r="D86" s="35" t="n">
+      <c r="C86" s="32"/>
+      <c r="D86" s="31" t="n">
         <f aca="false">(A86-1)*NBOXES+LBOX2</f>
         <v>222</v>
       </c>
-      <c r="E86" s="36"/>
-      <c r="F86" s="35" t="n">
+      <c r="E86" s="32"/>
+      <c r="F86" s="31" t="n">
         <f aca="false">(A86-1)*NBOXES+LBOX3</f>
         <v>223</v>
       </c>
-      <c r="G86" s="36"/>
-      <c r="H86" s="35" t="n">
+      <c r="G86" s="32"/>
+      <c r="H86" s="31" t="n">
         <f aca="false">(A86-1)*NBOXES+LBOX4</f>
         <v>224</v>
       </c>
-      <c r="I86" s="37"/>
+      <c r="I86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="30" t="n">
+      <c r="A87" s="27" t="n">
         <v>57</v>
       </c>
-      <c r="B87" s="35" t="n">
+      <c r="B87" s="31" t="n">
         <f aca="false">(A87-1)*NBOXES+LBOX1</f>
         <v>225</v>
       </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="35" t="n">
+      <c r="C87" s="32"/>
+      <c r="D87" s="31" t="n">
         <f aca="false">(A87-1)*NBOXES+LBOX2</f>
         <v>226</v>
       </c>
-      <c r="E87" s="36"/>
-      <c r="F87" s="35" t="n">
+      <c r="E87" s="32"/>
+      <c r="F87" s="31" t="n">
         <f aca="false">(A87-1)*NBOXES+LBOX3</f>
         <v>227</v>
       </c>
-      <c r="G87" s="36"/>
-      <c r="H87" s="35" t="n">
+      <c r="G87" s="32"/>
+      <c r="H87" s="31" t="n">
         <f aca="false">(A87-1)*NBOXES+LBOX4</f>
         <v>228</v>
       </c>
-      <c r="I87" s="37"/>
+      <c r="I87" s="32"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="34" t="n">
+      <c r="A88" s="30" t="n">
         <v>58</v>
       </c>
-      <c r="B88" s="35" t="n">
+      <c r="B88" s="31" t="n">
         <f aca="false">(A88-1)*NBOXES+LBOX1</f>
         <v>229</v>
       </c>
-      <c r="C88" s="36"/>
-      <c r="D88" s="35" t="n">
+      <c r="C88" s="32"/>
+      <c r="D88" s="31" t="n">
         <f aca="false">(A88-1)*NBOXES+LBOX2</f>
         <v>230</v>
       </c>
-      <c r="E88" s="36"/>
-      <c r="F88" s="35" t="n">
+      <c r="E88" s="32"/>
+      <c r="F88" s="31" t="n">
         <f aca="false">(A88-1)*NBOXES+LBOX3</f>
         <v>231</v>
       </c>
-      <c r="G88" s="36"/>
-      <c r="H88" s="35" t="n">
+      <c r="G88" s="32"/>
+      <c r="H88" s="31" t="n">
         <f aca="false">(A88-1)*NBOXES+LBOX4</f>
         <v>232</v>
       </c>
-      <c r="I88" s="37"/>
+      <c r="I88" s="32"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="30" t="n">
+      <c r="A89" s="27" t="n">
         <v>59</v>
       </c>
-      <c r="B89" s="35" t="n">
+      <c r="B89" s="31" t="n">
         <f aca="false">(A89-1)*NBOXES+LBOX1</f>
         <v>233</v>
       </c>
-      <c r="C89" s="37"/>
-      <c r="D89" s="35" t="n">
+      <c r="C89" s="32"/>
+      <c r="D89" s="31" t="n">
         <f aca="false">(A89-1)*NBOXES+LBOX2</f>
         <v>234</v>
       </c>
-      <c r="E89" s="37"/>
-      <c r="F89" s="35" t="n">
+      <c r="E89" s="32"/>
+      <c r="F89" s="31" t="n">
         <f aca="false">(A89-1)*NBOXES+LBOX3</f>
         <v>235</v>
       </c>
-      <c r="G89" s="37"/>
-      <c r="H89" s="35" t="n">
+      <c r="G89" s="32"/>
+      <c r="H89" s="31" t="n">
         <f aca="false">(A89-1)*NBOXES+LBOX4</f>
         <v>236</v>
       </c>
-      <c r="I89" s="37"/>
+      <c r="I89" s="32"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="38" t="n">
+      <c r="A90" s="33" t="n">
         <v>60</v>
       </c>
-      <c r="B90" s="39" t="n">
+      <c r="B90" s="34" t="n">
         <f aca="false">(A90-1)*NBOXES+LBOX1</f>
         <v>237</v>
       </c>
-      <c r="C90" s="40"/>
-      <c r="D90" s="39" t="n">
+      <c r="C90" s="35"/>
+      <c r="D90" s="34" t="n">
         <f aca="false">(A90-1)*NBOXES+LBOX2</f>
         <v>238</v>
       </c>
-      <c r="E90" s="40"/>
-      <c r="F90" s="39" t="n">
+      <c r="E90" s="35"/>
+      <c r="F90" s="34" t="n">
         <f aca="false">(A90-1)*NBOXES+LBOX3</f>
         <v>239</v>
       </c>
-      <c r="G90" s="40"/>
-      <c r="H90" s="39" t="n">
+      <c r="G90" s="35"/>
+      <c r="H90" s="34" t="n">
         <f aca="false">(A90-1)*NBOXES+LBOX4</f>
         <v>240</v>
       </c>
-      <c r="I90" s="45"/>
+      <c r="I90" s="35"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H91" s="43" t="s">
+      <c r="H91" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I91" s="44" t="n">
+      <c r="I91" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C79:I90)-LEN(SUBSTITUTE(UPPER(C79:I90),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="26" t="s">
+      <c r="A92" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B92" s="26" t="s">
+      <c r="B92" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C92" s="27"/>
+      <c r="C92" s="24"/>
     </row>
     <row r="93" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B93" s="28" t="s">
+      <c r="B93" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C93" s="29" t="s">
+      <c r="C93" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="28" t="s">
+      <c r="D93" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E93" s="29" t="s">
+      <c r="E93" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F93" s="28" t="s">
+      <c r="F93" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G93" s="29" t="s">
+      <c r="G93" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H93" s="28" t="s">
+      <c r="H93" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I93" s="29" t="s">
+      <c r="I93" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="46" t="n">
+      <c r="A94" s="40" t="n">
         <v>61</v>
       </c>
-      <c r="B94" s="31" t="n">
+      <c r="B94" s="28" t="n">
         <f aca="false">(A94-1)*NBOXES+LBOX1</f>
         <v>241</v>
       </c>
-      <c r="C94" s="32"/>
-      <c r="D94" s="31" t="n">
+      <c r="C94" s="29"/>
+      <c r="D94" s="28" t="n">
         <f aca="false">(A94-1)*NBOXES+LBOX2</f>
         <v>242</v>
       </c>
-      <c r="E94" s="32"/>
-      <c r="F94" s="31" t="n">
+      <c r="E94" s="29"/>
+      <c r="F94" s="28" t="n">
         <f aca="false">(A94-1)*NBOXES+LBOX3</f>
         <v>243</v>
       </c>
-      <c r="G94" s="32"/>
-      <c r="H94" s="31" t="n">
+      <c r="G94" s="29"/>
+      <c r="H94" s="28" t="n">
         <f aca="false">(A94-1)*NBOXES+LBOX4</f>
         <v>244</v>
       </c>
-      <c r="I94" s="33"/>
+      <c r="I94" s="29"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="34" t="n">
+      <c r="A95" s="30" t="n">
         <v>62</v>
       </c>
-      <c r="B95" s="35" t="n">
+      <c r="B95" s="31" t="n">
         <f aca="false">(A95-1)*NBOXES+LBOX1</f>
         <v>245</v>
       </c>
-      <c r="C95" s="36"/>
-      <c r="D95" s="35" t="n">
+      <c r="C95" s="32"/>
+      <c r="D95" s="31" t="n">
         <f aca="false">(A95-1)*NBOXES+LBOX2</f>
         <v>246</v>
       </c>
-      <c r="E95" s="36"/>
-      <c r="F95" s="35" t="n">
+      <c r="E95" s="32"/>
+      <c r="F95" s="31" t="n">
         <f aca="false">(A95-1)*NBOXES+LBOX3</f>
         <v>247</v>
       </c>
-      <c r="G95" s="36"/>
-      <c r="H95" s="35" t="n">
+      <c r="G95" s="32"/>
+      <c r="H95" s="31" t="n">
         <f aca="false">(A95-1)*NBOXES+LBOX4</f>
         <v>248</v>
       </c>
-      <c r="I95" s="37"/>
+      <c r="I95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="30" t="n">
+      <c r="A96" s="27" t="n">
         <v>63</v>
       </c>
-      <c r="B96" s="35" t="n">
+      <c r="B96" s="31" t="n">
         <f aca="false">(A96-1)*NBOXES+LBOX1</f>
         <v>249</v>
       </c>
-      <c r="C96" s="36"/>
-      <c r="D96" s="35" t="n">
+      <c r="C96" s="32"/>
+      <c r="D96" s="31" t="n">
         <f aca="false">(A96-1)*NBOXES+LBOX2</f>
         <v>250</v>
       </c>
-      <c r="E96" s="36"/>
-      <c r="F96" s="35" t="n">
+      <c r="E96" s="32"/>
+      <c r="F96" s="31" t="n">
         <f aca="false">(A96-1)*NBOXES+LBOX3</f>
         <v>251</v>
       </c>
-      <c r="G96" s="36"/>
-      <c r="H96" s="35" t="n">
+      <c r="G96" s="32"/>
+      <c r="H96" s="31" t="n">
         <f aca="false">(A96-1)*NBOXES+LBOX4</f>
         <v>252</v>
       </c>
-      <c r="I96" s="37"/>
+      <c r="I96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="34" t="n">
+      <c r="A97" s="30" t="n">
         <v>64</v>
       </c>
-      <c r="B97" s="35" t="n">
+      <c r="B97" s="31" t="n">
         <f aca="false">(A97-1)*NBOXES+LBOX1</f>
         <v>253</v>
       </c>
-      <c r="C97" s="36"/>
-      <c r="D97" s="35" t="n">
+      <c r="C97" s="32"/>
+      <c r="D97" s="31" t="n">
         <f aca="false">(A97-1)*NBOXES+LBOX2</f>
         <v>254</v>
       </c>
-      <c r="E97" s="36"/>
-      <c r="F97" s="35" t="n">
+      <c r="E97" s="32"/>
+      <c r="F97" s="31" t="n">
         <f aca="false">(A97-1)*NBOXES+LBOX3</f>
         <v>255</v>
       </c>
-      <c r="G97" s="36"/>
-      <c r="H97" s="35" t="n">
+      <c r="G97" s="32"/>
+      <c r="H97" s="31" t="n">
         <f aca="false">(A97-1)*NBOXES+LBOX4</f>
         <v>256</v>
       </c>
-      <c r="I97" s="37"/>
+      <c r="I97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="30" t="n">
+      <c r="A98" s="27" t="n">
         <v>65</v>
       </c>
-      <c r="B98" s="35" t="n">
+      <c r="B98" s="31" t="n">
         <f aca="false">(A98-1)*NBOXES+LBOX1</f>
         <v>257</v>
       </c>
-      <c r="C98" s="36"/>
-      <c r="D98" s="35" t="n">
+      <c r="C98" s="32"/>
+      <c r="D98" s="31" t="n">
         <f aca="false">(A98-1)*NBOXES+LBOX2</f>
         <v>258</v>
       </c>
-      <c r="E98" s="36"/>
-      <c r="F98" s="35" t="n">
+      <c r="E98" s="32"/>
+      <c r="F98" s="31" t="n">
         <f aca="false">(A98-1)*NBOXES+LBOX3</f>
         <v>259</v>
       </c>
-      <c r="G98" s="36"/>
-      <c r="H98" s="35" t="n">
+      <c r="G98" s="32"/>
+      <c r="H98" s="31" t="n">
         <f aca="false">(A98-1)*NBOXES+LBOX4</f>
         <v>260</v>
       </c>
-      <c r="I98" s="37"/>
+      <c r="I98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="34" t="n">
+      <c r="A99" s="30" t="n">
         <v>66</v>
       </c>
-      <c r="B99" s="35" t="n">
+      <c r="B99" s="31" t="n">
         <f aca="false">(A99-1)*NBOXES+LBOX1</f>
         <v>261</v>
       </c>
-      <c r="C99" s="36"/>
-      <c r="D99" s="35" t="n">
+      <c r="C99" s="32"/>
+      <c r="D99" s="31" t="n">
         <f aca="false">(A99-1)*NBOXES+LBOX2</f>
         <v>262</v>
       </c>
-      <c r="E99" s="36"/>
-      <c r="F99" s="35" t="n">
+      <c r="E99" s="32"/>
+      <c r="F99" s="31" t="n">
         <f aca="false">(A99-1)*NBOXES+LBOX3</f>
         <v>263</v>
       </c>
-      <c r="G99" s="36"/>
-      <c r="H99" s="35" t="n">
+      <c r="G99" s="32"/>
+      <c r="H99" s="31" t="n">
         <f aca="false">(A99-1)*NBOXES+LBOX4</f>
         <v>264</v>
       </c>
-      <c r="I99" s="37"/>
+      <c r="I99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="30" t="n">
+      <c r="A100" s="27" t="n">
         <v>67</v>
       </c>
-      <c r="B100" s="35" t="n">
+      <c r="B100" s="31" t="n">
         <f aca="false">(A100-1)*NBOXES+LBOX1</f>
         <v>265</v>
       </c>
-      <c r="C100" s="36"/>
-      <c r="D100" s="35" t="n">
+      <c r="C100" s="32"/>
+      <c r="D100" s="31" t="n">
         <f aca="false">(A100-1)*NBOXES+LBOX2</f>
         <v>266</v>
       </c>
-      <c r="E100" s="36"/>
-      <c r="F100" s="35" t="n">
+      <c r="E100" s="32"/>
+      <c r="F100" s="31" t="n">
         <f aca="false">(A100-1)*NBOXES+LBOX3</f>
         <v>267</v>
       </c>
-      <c r="G100" s="36"/>
-      <c r="H100" s="35" t="n">
+      <c r="G100" s="32"/>
+      <c r="H100" s="31" t="n">
         <f aca="false">(A100-1)*NBOXES+LBOX4</f>
         <v>268</v>
       </c>
-      <c r="I100" s="37"/>
+      <c r="I100" s="32"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="34" t="n">
+      <c r="A101" s="30" t="n">
         <v>68</v>
       </c>
-      <c r="B101" s="35" t="n">
+      <c r="B101" s="31" t="n">
         <f aca="false">(A101-1)*NBOXES+LBOX1</f>
         <v>269</v>
       </c>
-      <c r="C101" s="36"/>
-      <c r="D101" s="35" t="n">
+      <c r="C101" s="32"/>
+      <c r="D101" s="31" t="n">
         <f aca="false">(A101-1)*NBOXES+LBOX2</f>
         <v>270</v>
       </c>
-      <c r="E101" s="36"/>
-      <c r="F101" s="35" t="n">
+      <c r="E101" s="32"/>
+      <c r="F101" s="31" t="n">
         <f aca="false">(A101-1)*NBOXES+LBOX3</f>
         <v>271</v>
       </c>
-      <c r="G101" s="36"/>
-      <c r="H101" s="35" t="n">
+      <c r="G101" s="32"/>
+      <c r="H101" s="31" t="n">
         <f aca="false">(A101-1)*NBOXES+LBOX4</f>
         <v>272</v>
       </c>
-      <c r="I101" s="37"/>
+      <c r="I101" s="32"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="30" t="n">
+      <c r="A102" s="27" t="n">
         <v>69</v>
       </c>
-      <c r="B102" s="35" t="n">
+      <c r="B102" s="31" t="n">
         <f aca="false">(A102-1)*NBOXES+LBOX1</f>
         <v>273</v>
       </c>
-      <c r="C102" s="36"/>
-      <c r="D102" s="35" t="n">
+      <c r="C102" s="32"/>
+      <c r="D102" s="31" t="n">
         <f aca="false">(A102-1)*NBOXES+LBOX2</f>
         <v>274</v>
       </c>
-      <c r="E102" s="36"/>
-      <c r="F102" s="35" t="n">
+      <c r="E102" s="32"/>
+      <c r="F102" s="31" t="n">
         <f aca="false">(A102-1)*NBOXES+LBOX3</f>
         <v>275</v>
       </c>
-      <c r="G102" s="36"/>
-      <c r="H102" s="35" t="n">
+      <c r="G102" s="32"/>
+      <c r="H102" s="31" t="n">
         <f aca="false">(A102-1)*NBOXES+LBOX4</f>
         <v>276</v>
       </c>
-      <c r="I102" s="37"/>
+      <c r="I102" s="32"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="34" t="n">
+      <c r="A103" s="30" t="n">
         <v>70</v>
       </c>
-      <c r="B103" s="35" t="n">
+      <c r="B103" s="31" t="n">
         <f aca="false">(A103-1)*NBOXES+LBOX1</f>
         <v>277</v>
       </c>
-      <c r="C103" s="36"/>
-      <c r="D103" s="35" t="n">
+      <c r="C103" s="32"/>
+      <c r="D103" s="31" t="n">
         <f aca="false">(A103-1)*NBOXES+LBOX2</f>
         <v>278</v>
       </c>
-      <c r="E103" s="36"/>
-      <c r="F103" s="35" t="n">
+      <c r="E103" s="32"/>
+      <c r="F103" s="31" t="n">
         <f aca="false">(A103-1)*NBOXES+LBOX3</f>
         <v>279</v>
       </c>
-      <c r="G103" s="36"/>
-      <c r="H103" s="35" t="n">
+      <c r="G103" s="32"/>
+      <c r="H103" s="31" t="n">
         <f aca="false">(A103-1)*NBOXES+LBOX4</f>
         <v>280</v>
       </c>
-      <c r="I103" s="37"/>
+      <c r="I103" s="32"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="30" t="n">
+      <c r="A104" s="27" t="n">
         <v>71</v>
       </c>
-      <c r="B104" s="35" t="n">
+      <c r="B104" s="31" t="n">
         <f aca="false">(A104-1)*NBOXES+LBOX1</f>
         <v>281</v>
       </c>
-      <c r="C104" s="37"/>
-      <c r="D104" s="35" t="n">
+      <c r="C104" s="32"/>
+      <c r="D104" s="31" t="n">
         <f aca="false">(A104-1)*NBOXES+LBOX2</f>
         <v>282</v>
       </c>
-      <c r="E104" s="37"/>
-      <c r="F104" s="35" t="n">
+      <c r="E104" s="32"/>
+      <c r="F104" s="31" t="n">
         <f aca="false">(A104-1)*NBOXES+LBOX3</f>
         <v>283</v>
       </c>
-      <c r="G104" s="37"/>
-      <c r="H104" s="35" t="n">
+      <c r="G104" s="32"/>
+      <c r="H104" s="31" t="n">
         <f aca="false">(A104-1)*NBOXES+LBOX4</f>
         <v>284</v>
       </c>
-      <c r="I104" s="37"/>
+      <c r="I104" s="32"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="38" t="n">
+      <c r="A105" s="33" t="n">
         <v>72</v>
       </c>
-      <c r="B105" s="39" t="n">
+      <c r="B105" s="34" t="n">
         <f aca="false">(A105-1)*NBOXES+LBOX1</f>
         <v>285</v>
       </c>
-      <c r="C105" s="40"/>
-      <c r="D105" s="39" t="n">
+      <c r="C105" s="35"/>
+      <c r="D105" s="34" t="n">
         <f aca="false">(A105-1)*NBOXES+LBOX2</f>
         <v>286</v>
       </c>
-      <c r="E105" s="40"/>
-      <c r="F105" s="39" t="n">
+      <c r="E105" s="35"/>
+      <c r="F105" s="34" t="n">
         <f aca="false">(A105-1)*NBOXES+LBOX3</f>
         <v>287</v>
       </c>
-      <c r="G105" s="40"/>
-      <c r="H105" s="39" t="n">
+      <c r="G105" s="35"/>
+      <c r="H105" s="34" t="n">
         <f aca="false">(A105-1)*NBOXES+LBOX4</f>
         <v>288</v>
       </c>
-      <c r="I105" s="45"/>
+      <c r="I105" s="35"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H106" s="43" t="s">
+      <c r="H106" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I106" s="44" t="n">
+      <c r="I106" s="39" t="n">
         <f aca="false">SUMPRODUCT(LEN(C94:I105)-LEN(SUBSTITUTE(UPPER(C94:I105),"X","")))</f>
         <v>0</v>
       </c>
@@ -3450,7 +3210,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="47" t="s">
+      <c r="B110" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -3458,7 +3218,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="47" t="s">
+      <c r="B111" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -3466,7 +3226,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="47" t="s">
+      <c r="B112" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C112" s="1" t="s">

</xml_diff>

<commit_message>
xs-TAINI-laser1: add checks for non-numeric subject IDs xs-ldas-XLASER1: finish evoked potential analysis - started power xs-ldas-coh1/xs-ldas-pow1: remove setting for --fhi, as this is only an option for matrixmerge xs-ldas-XLASER1: rename option --fhi to --evhi to clarify that it is applied to the evoked-potential output update laser tworksheet template to discount empty SUBJECT-ID boxes xe-align2.10.c: minor fix
</commit_message>
<xml_diff>
--- a/docs/templates/template_taini_worksheet_laser.xlsx
+++ b/docs/templates/template_taini_worksheet_laser.xlsx
@@ -301,10 +301,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -626,11 +627,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,7 +659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -674,7 +675,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,7 +687,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -698,7 +699,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,7 +707,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,7 +719,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,12 +733,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -909,11 +910,11 @@
   </sheetPr>
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.13"/>
@@ -924,7 +925,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,22 +1026,22 @@
         <v>4</v>
       </c>
       <c r="C9" s="17" t="n">
-        <f aca="false">IF(SUBJECT1&gt;0,1,0)</f>
+        <f aca="false">IF(SUBJECT1="",0,1)</f>
         <v>1</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17" t="n">
-        <f aca="false">IF(SUBJECT2&gt;0,1,0)</f>
+        <f aca="false">IF(SUBJECT2="",0,1)</f>
         <v>1</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17" t="n">
-        <f aca="false">IF(SUBJECT3&gt;0,1,0)</f>
+        <f aca="false">IF(SUBJECT3="",0,1)</f>
         <v>1</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17" t="n">
-        <f aca="false">IF(SUBJECT4&gt;0,1,0)</f>
+        <f aca="false">IF(SUBJECT4="",0,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1048,9 +1049,7 @@
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="18" t="n">
-        <v>1</v>
-      </c>
+      <c r="C10" s="18"/>
       <c r="D10" s="19"/>
       <c r="E10" s="18" t="n">
         <v>2</v>
@@ -1131,7 +1130,7 @@
       </c>
       <c r="B15" s="28" t="n">
         <f aca="false">(A15-1)*NBOXES+LBOX1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="28" t="n">
@@ -1159,7 +1158,7 @@
       </c>
       <c r="B16" s="31" t="n">
         <f aca="false">(A16-1)*NBOXES+LBOX1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="31" t="n">
@@ -1187,7 +1186,7 @@
       </c>
       <c r="B17" s="31" t="n">
         <f aca="false">(A17-1)*NBOXES+LBOX1</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="31" t="n">
@@ -1213,7 +1212,7 @@
       </c>
       <c r="B18" s="31" t="n">
         <f aca="false">(A18-1)*NBOXES+LBOX1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="31" t="n">
@@ -1240,7 +1239,7 @@
       </c>
       <c r="B19" s="31" t="n">
         <f aca="false">(A19-1)*NBOXES+LBOX1</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="31" t="n">
@@ -1267,7 +1266,7 @@
       </c>
       <c r="B20" s="31" t="n">
         <f aca="false">(A20-1)*NBOXES+LBOX1</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="31" t="n">
@@ -1299,7 +1298,7 @@
       </c>
       <c r="B21" s="31" t="n">
         <f aca="false">(A21-1)*NBOXES+LBOX1</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="31" t="n">
@@ -1328,7 +1327,7 @@
       </c>
       <c r="B22" s="31" t="n">
         <f aca="false">(A22-1)*NBOXES+LBOX1</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="31" t="n">
@@ -1354,7 +1353,7 @@
       </c>
       <c r="B23" s="31" t="n">
         <f aca="false">(A23-1)*NBOXES+LBOX1</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="31" t="n">
@@ -1386,7 +1385,7 @@
       </c>
       <c r="B24" s="31" t="n">
         <f aca="false">(A24-1)*NBOXES+LBOX1</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="32"/>
       <c r="D24" s="31" t="n">
@@ -1411,7 +1410,7 @@
       </c>
       <c r="B25" s="31" t="n">
         <f aca="false">(A25-1)*NBOXES+LBOX1</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="32"/>
       <c r="D25" s="31" t="n">
@@ -1436,7 +1435,7 @@
       </c>
       <c r="B26" s="34" t="n">
         <f aca="false">(A26-1)*NBOXES+LBOX1</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="34" t="n">
@@ -1510,7 +1509,7 @@
       </c>
       <c r="B30" s="28" t="n">
         <f aca="false">(A30-1)*NBOXES+LBOX1</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="28" t="n">
@@ -1535,7 +1534,7 @@
       </c>
       <c r="B31" s="31" t="n">
         <f aca="false">(A31-1)*NBOXES+LBOX1</f>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="31" t="n">
@@ -1560,7 +1559,7 @@
       </c>
       <c r="B32" s="31" t="n">
         <f aca="false">(A32-1)*NBOXES+LBOX1</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="31" t="n">
@@ -1585,7 +1584,7 @@
       </c>
       <c r="B33" s="31" t="n">
         <f aca="false">(A33-1)*NBOXES+LBOX1</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="31" t="n">
@@ -1610,7 +1609,7 @@
       </c>
       <c r="B34" s="31" t="n">
         <f aca="false">(A34-1)*NBOXES+LBOX1</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="31" t="n">
@@ -1635,7 +1634,7 @@
       </c>
       <c r="B35" s="31" t="n">
         <f aca="false">(A35-1)*NBOXES+LBOX1</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="32"/>
       <c r="D35" s="31" t="n">
@@ -1660,7 +1659,7 @@
       </c>
       <c r="B36" s="31" t="n">
         <f aca="false">(A36-1)*NBOXES+LBOX1</f>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="31" t="n">
@@ -1685,7 +1684,7 @@
       </c>
       <c r="B37" s="31" t="n">
         <f aca="false">(A37-1)*NBOXES+LBOX1</f>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="32"/>
       <c r="D37" s="31" t="n">
@@ -1710,7 +1709,7 @@
       </c>
       <c r="B38" s="31" t="n">
         <f aca="false">(A38-1)*NBOXES+LBOX1</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="32"/>
       <c r="D38" s="31" t="n">
@@ -1735,7 +1734,7 @@
       </c>
       <c r="B39" s="31" t="n">
         <f aca="false">(A39-1)*NBOXES+LBOX1</f>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="32"/>
       <c r="D39" s="31" t="n">
@@ -1760,7 +1759,7 @@
       </c>
       <c r="B40" s="31" t="n">
         <f aca="false">(A40-1)*NBOXES+LBOX1</f>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="32"/>
       <c r="D40" s="31" t="n">
@@ -1785,7 +1784,7 @@
       </c>
       <c r="B41" s="34" t="n">
         <f aca="false">(A41-1)*NBOXES+LBOX1</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="35"/>
       <c r="D41" s="34" t="n">
@@ -1857,7 +1856,7 @@
       </c>
       <c r="B45" s="28" t="n">
         <f aca="false">(A45-1)*NBOXES+LBOX1</f>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="29"/>
       <c r="D45" s="28" t="n">
@@ -1882,7 +1881,7 @@
       </c>
       <c r="B46" s="31" t="n">
         <f aca="false">(A46-1)*NBOXES+LBOX1</f>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="32"/>
       <c r="D46" s="31" t="n">
@@ -1907,7 +1906,7 @@
       </c>
       <c r="B47" s="31" t="n">
         <f aca="false">(A47-1)*NBOXES+LBOX1</f>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" s="32"/>
       <c r="D47" s="31" t="n">
@@ -1932,7 +1931,7 @@
       </c>
       <c r="B48" s="31" t="n">
         <f aca="false">(A48-1)*NBOXES+LBOX1</f>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="32"/>
       <c r="D48" s="31" t="n">
@@ -1957,7 +1956,7 @@
       </c>
       <c r="B49" s="31" t="n">
         <f aca="false">(A49-1)*NBOXES+LBOX1</f>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C49" s="32"/>
       <c r="D49" s="31" t="n">
@@ -1982,7 +1981,7 @@
       </c>
       <c r="B50" s="31" t="n">
         <f aca="false">(A50-1)*NBOXES+LBOX1</f>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50" s="32"/>
       <c r="D50" s="31" t="n">
@@ -2007,7 +2006,7 @@
       </c>
       <c r="B51" s="31" t="n">
         <f aca="false">(A51-1)*NBOXES+LBOX1</f>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C51" s="32"/>
       <c r="D51" s="31" t="n">
@@ -2032,7 +2031,7 @@
       </c>
       <c r="B52" s="31" t="n">
         <f aca="false">(A52-1)*NBOXES+LBOX1</f>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C52" s="32"/>
       <c r="D52" s="31" t="n">
@@ -2057,7 +2056,7 @@
       </c>
       <c r="B53" s="31" t="n">
         <f aca="false">(A53-1)*NBOXES+LBOX1</f>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C53" s="32"/>
       <c r="D53" s="31" t="n">
@@ -2082,7 +2081,7 @@
       </c>
       <c r="B54" s="31" t="n">
         <f aca="false">(A54-1)*NBOXES+LBOX1</f>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C54" s="32"/>
       <c r="D54" s="31" t="n">
@@ -2107,7 +2106,7 @@
       </c>
       <c r="B55" s="31" t="n">
         <f aca="false">(A55-1)*NBOXES+LBOX1</f>
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C55" s="32"/>
       <c r="D55" s="31" t="n">
@@ -2132,7 +2131,7 @@
       </c>
       <c r="B56" s="34" t="n">
         <f aca="false">(A56-1)*NBOXES+LBOX1</f>
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C56" s="35"/>
       <c r="D56" s="34" t="n">
@@ -2204,7 +2203,7 @@
       </c>
       <c r="B64" s="28" t="n">
         <f aca="false">(A64-1)*NBOXES+LBOX1</f>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="29"/>
       <c r="D64" s="28" t="n">
@@ -2229,7 +2228,7 @@
       </c>
       <c r="B65" s="31" t="n">
         <f aca="false">(A65-1)*NBOXES+LBOX1</f>
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" s="32"/>
       <c r="D65" s="31" t="n">
@@ -2254,7 +2253,7 @@
       </c>
       <c r="B66" s="31" t="n">
         <f aca="false">(A66-1)*NBOXES+LBOX1</f>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C66" s="32"/>
       <c r="D66" s="31" t="n">
@@ -2279,7 +2278,7 @@
       </c>
       <c r="B67" s="31" t="n">
         <f aca="false">(A67-1)*NBOXES+LBOX1</f>
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C67" s="32"/>
       <c r="D67" s="31" t="n">
@@ -2304,7 +2303,7 @@
       </c>
       <c r="B68" s="31" t="n">
         <f aca="false">(A68-1)*NBOXES+LBOX1</f>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C68" s="32"/>
       <c r="D68" s="31" t="n">
@@ -2329,7 +2328,7 @@
       </c>
       <c r="B69" s="31" t="n">
         <f aca="false">(A69-1)*NBOXES+LBOX1</f>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C69" s="32"/>
       <c r="D69" s="31" t="n">
@@ -2354,7 +2353,7 @@
       </c>
       <c r="B70" s="31" t="n">
         <f aca="false">(A70-1)*NBOXES+LBOX1</f>
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C70" s="32"/>
       <c r="D70" s="31" t="n">
@@ -2379,7 +2378,7 @@
       </c>
       <c r="B71" s="31" t="n">
         <f aca="false">(A71-1)*NBOXES+LBOX1</f>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C71" s="32"/>
       <c r="D71" s="31" t="n">
@@ -2404,7 +2403,7 @@
       </c>
       <c r="B72" s="31" t="n">
         <f aca="false">(A72-1)*NBOXES+LBOX1</f>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="31" t="n">
@@ -2429,7 +2428,7 @@
       </c>
       <c r="B73" s="31" t="n">
         <f aca="false">(A73-1)*NBOXES+LBOX1</f>
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C73" s="32"/>
       <c r="D73" s="31" t="n">
@@ -2454,7 +2453,7 @@
       </c>
       <c r="B74" s="31" t="n">
         <f aca="false">(A74-1)*NBOXES+LBOX1</f>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C74" s="32"/>
       <c r="D74" s="31" t="n">
@@ -2479,7 +2478,7 @@
       </c>
       <c r="B75" s="34" t="n">
         <f aca="false">(A75-1)*NBOXES+LBOX1</f>
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C75" s="35"/>
       <c r="D75" s="34" t="n">
@@ -2551,7 +2550,7 @@
       </c>
       <c r="B79" s="28" t="n">
         <f aca="false">(A79-1)*NBOXES+LBOX1</f>
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="28" t="n">
@@ -2576,7 +2575,7 @@
       </c>
       <c r="B80" s="31" t="n">
         <f aca="false">(A80-1)*NBOXES+LBOX1</f>
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C80" s="32"/>
       <c r="D80" s="31" t="n">
@@ -2601,7 +2600,7 @@
       </c>
       <c r="B81" s="31" t="n">
         <f aca="false">(A81-1)*NBOXES+LBOX1</f>
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C81" s="32"/>
       <c r="D81" s="31" t="n">
@@ -2626,7 +2625,7 @@
       </c>
       <c r="B82" s="31" t="n">
         <f aca="false">(A82-1)*NBOXES+LBOX1</f>
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C82" s="32"/>
       <c r="D82" s="31" t="n">
@@ -2651,7 +2650,7 @@
       </c>
       <c r="B83" s="31" t="n">
         <f aca="false">(A83-1)*NBOXES+LBOX1</f>
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C83" s="32"/>
       <c r="D83" s="31" t="n">
@@ -2676,7 +2675,7 @@
       </c>
       <c r="B84" s="31" t="n">
         <f aca="false">(A84-1)*NBOXES+LBOX1</f>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C84" s="32"/>
       <c r="D84" s="31" t="n">
@@ -2701,7 +2700,7 @@
       </c>
       <c r="B85" s="31" t="n">
         <f aca="false">(A85-1)*NBOXES+LBOX1</f>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="31" t="n">
@@ -2726,7 +2725,7 @@
       </c>
       <c r="B86" s="31" t="n">
         <f aca="false">(A86-1)*NBOXES+LBOX1</f>
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C86" s="32"/>
       <c r="D86" s="31" t="n">
@@ -2751,7 +2750,7 @@
       </c>
       <c r="B87" s="31" t="n">
         <f aca="false">(A87-1)*NBOXES+LBOX1</f>
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C87" s="32"/>
       <c r="D87" s="31" t="n">
@@ -2776,7 +2775,7 @@
       </c>
       <c r="B88" s="31" t="n">
         <f aca="false">(A88-1)*NBOXES+LBOX1</f>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C88" s="32"/>
       <c r="D88" s="31" t="n">
@@ -2801,7 +2800,7 @@
       </c>
       <c r="B89" s="31" t="n">
         <f aca="false">(A89-1)*NBOXES+LBOX1</f>
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C89" s="32"/>
       <c r="D89" s="31" t="n">
@@ -2826,7 +2825,7 @@
       </c>
       <c r="B90" s="34" t="n">
         <f aca="false">(A90-1)*NBOXES+LBOX1</f>
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C90" s="35"/>
       <c r="D90" s="34" t="n">
@@ -2898,7 +2897,7 @@
       </c>
       <c r="B94" s="28" t="n">
         <f aca="false">(A94-1)*NBOXES+LBOX1</f>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C94" s="29"/>
       <c r="D94" s="28" t="n">
@@ -2923,7 +2922,7 @@
       </c>
       <c r="B95" s="31" t="n">
         <f aca="false">(A95-1)*NBOXES+LBOX1</f>
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C95" s="32"/>
       <c r="D95" s="31" t="n">
@@ -2948,7 +2947,7 @@
       </c>
       <c r="B96" s="31" t="n">
         <f aca="false">(A96-1)*NBOXES+LBOX1</f>
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C96" s="32"/>
       <c r="D96" s="31" t="n">
@@ -2973,7 +2972,7 @@
       </c>
       <c r="B97" s="31" t="n">
         <f aca="false">(A97-1)*NBOXES+LBOX1</f>
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C97" s="32"/>
       <c r="D97" s="31" t="n">
@@ -2998,7 +2997,7 @@
       </c>
       <c r="B98" s="31" t="n">
         <f aca="false">(A98-1)*NBOXES+LBOX1</f>
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C98" s="32"/>
       <c r="D98" s="31" t="n">
@@ -3023,7 +3022,7 @@
       </c>
       <c r="B99" s="31" t="n">
         <f aca="false">(A99-1)*NBOXES+LBOX1</f>
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C99" s="32"/>
       <c r="D99" s="31" t="n">
@@ -3048,7 +3047,7 @@
       </c>
       <c r="B100" s="31" t="n">
         <f aca="false">(A100-1)*NBOXES+LBOX1</f>
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C100" s="32"/>
       <c r="D100" s="31" t="n">
@@ -3073,7 +3072,7 @@
       </c>
       <c r="B101" s="31" t="n">
         <f aca="false">(A101-1)*NBOXES+LBOX1</f>
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C101" s="32"/>
       <c r="D101" s="31" t="n">
@@ -3098,7 +3097,7 @@
       </c>
       <c r="B102" s="31" t="n">
         <f aca="false">(A102-1)*NBOXES+LBOX1</f>
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C102" s="32"/>
       <c r="D102" s="31" t="n">
@@ -3123,7 +3122,7 @@
       </c>
       <c r="B103" s="31" t="n">
         <f aca="false">(A103-1)*NBOXES+LBOX1</f>
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C103" s="32"/>
       <c r="D103" s="31" t="n">
@@ -3148,7 +3147,7 @@
       </c>
       <c r="B104" s="31" t="n">
         <f aca="false">(A104-1)*NBOXES+LBOX1</f>
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C104" s="32"/>
       <c r="D104" s="31" t="n">
@@ -3173,7 +3172,7 @@
       </c>
       <c r="B105" s="34" t="n">
         <f aca="false">(A105-1)*NBOXES+LBOX1</f>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C105" s="35"/>
       <c r="D105" s="34" t="n">

</xml_diff>

<commit_message>
Update laser workesheet comments
</commit_message>
<xml_diff>
--- a/docs/templates/template_taini_worksheet_laser.xlsx
+++ b/docs/templates/template_taini_worksheet_laser.xlsx
@@ -40,7 +40,6 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
     <author>John</author>
   </authors>
   <commentList>
@@ -48,11 +47,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The  TAINI config .yaml file corresponding to this recording session
 Example:
@@ -66,11 +64,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t>Optional name of the experimenter.</t>
         </r>
@@ -80,14 +77,14 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t>The date this session was recorded. Format: dd/mm/yyy. Example:
-25/12/2020</t>
+          <t>The date this session was recorded. 
+Format: dd/mm/yyy
+Example: 25/12/2020</t>
         </r>
       </text>
     </comment>
@@ -95,11 +92,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t>The laser spot size
 Example: 4 mm</t>
@@ -110,11 +106,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t>The laser pulse duration
 Example: 4ms</t>
@@ -125,11 +120,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Numeric values, must be greater than zero. 
 Leave blank to grey-out the box. 
@@ -142,11 +136,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t>Enter the stimulus strength for this block of trials. 
 Example: 1.50
@@ -155,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="1">
+    <comment ref="B15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="1">
+    <comment ref="C15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -716,18 +709,6 @@
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -839,179 +820,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill>
@@ -1687,6 +1512,342 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9315450" cy="9286875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1980,28 +2141,28 @@
   <dimension ref="A1:AMK114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C15" sqref="C15:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" customWidth="1"/>
-    <col min="10" max="1025" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
+    <col min="10" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="6"/>
+      <c r="I1" s="3"/>
       <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
@@ -2012,11 +2173,11 @@
       <c r="R1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2"/>
-      <c r="I2" s="6"/>
+      <c r="I2" s="3"/>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
@@ -2027,334 +2188,334 @@
       <c r="R2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="10"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <f>SUM(C9,E9,G9,I9)</f>
         <v>4</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="14">
         <f>IF(SUBJECT1="",0,1)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14">
         <f>IF(SUBJECT2="",0,1)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14">
         <f>IF(SUBJECT3="",0,1)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
         <f>IF(SUBJECT4="",0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="15">
         <v>1</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="18">
+      <c r="D10" s="16"/>
+      <c r="E10" s="15">
         <v>2</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18">
+      <c r="F10" s="16"/>
+      <c r="G10" s="15">
         <v>3</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="15">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="19"/>
+      <c r="G11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="21" t="s">
+      <c r="H11" s="19"/>
+      <c r="I11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="14" spans="1:19" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="S14"/>
     </row>
     <row r="15" spans="1:19" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="24">
         <v>1</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="39">
         <f>ACTIVE1</f>
         <v>1</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42">
-        <f>B15+ACTIVE1</f>
+      <c r="C15" s="40"/>
+      <c r="D15" s="39">
+        <f t="shared" ref="D15:D26" si="0">B15+ACTIVE1</f>
         <v>2</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="42">
-        <f>D15+ACTIVE2</f>
+      <c r="E15" s="40"/>
+      <c r="F15" s="39">
+        <f t="shared" ref="F15:F26" si="1">D15+ACTIVE2</f>
         <v>3</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="42">
-        <f>F15+ACTIVE3</f>
+      <c r="G15" s="40"/>
+      <c r="H15" s="39">
+        <f t="shared" ref="H15:H26" si="2">F15+ACTIVE3</f>
         <v>4</v>
       </c>
-      <c r="I15" s="43"/>
+      <c r="I15" s="40"/>
       <c r="L15"/>
       <c r="R15"/>
       <c r="S15"/>
     </row>
     <row r="16" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="27">
         <v>2</v>
       </c>
-      <c r="B16" s="31">
-        <f>H15+ACTIVE4</f>
+      <c r="B16" s="28">
+        <f t="shared" ref="B16:B26" si="3">H15+ACTIVE4</f>
         <v>5</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="28">
-        <f>B16+ACTIVE1</f>
+      <c r="C16" s="29"/>
+      <c r="D16" s="25">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="28">
-        <f>D16+ACTIVE2</f>
+      <c r="E16" s="29"/>
+      <c r="F16" s="25">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="28">
-        <f>F16+ACTIVE3</f>
+      <c r="G16" s="29"/>
+      <c r="H16" s="25">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="I16" s="32"/>
+      <c r="I16" s="29"/>
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
     </row>
     <row r="17" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="27">
         <v>3</v>
       </c>
-      <c r="B17" s="31">
-        <f>H16+ACTIVE4</f>
+      <c r="B17" s="28">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="28">
-        <f>B17+ACTIVE1</f>
+      <c r="C17" s="29"/>
+      <c r="D17" s="25">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="28">
-        <f>D17+ACTIVE2</f>
+      <c r="E17" s="29"/>
+      <c r="F17" s="25">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="28">
-        <f>F17+ACTIVE3</f>
+      <c r="G17" s="29"/>
+      <c r="H17" s="25">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I17" s="32"/>
+      <c r="I17" s="29"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="27">
         <v>4</v>
       </c>
-      <c r="B18" s="31">
-        <f>H17+ACTIVE4</f>
+      <c r="B18" s="28">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="28">
-        <f>B18+ACTIVE1</f>
+      <c r="C18" s="29"/>
+      <c r="D18" s="25">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="28">
-        <f>D18+ACTIVE2</f>
+      <c r="E18" s="29"/>
+      <c r="F18" s="25">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="28">
-        <f>F18+ACTIVE3</f>
+      <c r="G18" s="29"/>
+      <c r="H18" s="25">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="29"/>
       <c r="K18"/>
       <c r="R18"/>
     </row>
     <row r="19" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="27">
         <v>5</v>
       </c>
-      <c r="B19" s="31">
-        <f>H18+ACTIVE4</f>
+      <c r="B19" s="28">
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="28">
-        <f>B19+ACTIVE1</f>
+      <c r="C19" s="29"/>
+      <c r="D19" s="25">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="28">
-        <f>D19+ACTIVE2</f>
+      <c r="E19" s="29"/>
+      <c r="F19" s="25">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="28">
-        <f>F19+ACTIVE3</f>
+      <c r="G19" s="29"/>
+      <c r="H19" s="25">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="29"/>
       <c r="N19"/>
       <c r="O19"/>
     </row>
     <row r="20" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="27">
         <v>6</v>
       </c>
-      <c r="B20" s="31">
-        <f>H19+ACTIVE4</f>
+      <c r="B20" s="28">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="28">
-        <f>B20+ACTIVE1</f>
+      <c r="C20" s="29"/>
+      <c r="D20" s="25">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="28">
-        <f>D20+ACTIVE2</f>
+      <c r="E20" s="29"/>
+      <c r="F20" s="25">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="28">
-        <f>F20+ACTIVE3</f>
+      <c r="G20" s="29"/>
+      <c r="H20" s="25">
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="I20" s="32"/>
+      <c r="I20" s="29"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
@@ -2364,84 +2525,84 @@
       <c r="S20"/>
     </row>
     <row r="21" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="27">
         <v>7</v>
       </c>
-      <c r="B21" s="31">
-        <f>H20+ACTIVE4</f>
+      <c r="B21" s="28">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="28">
-        <f>B21+ACTIVE1</f>
+      <c r="C21" s="29"/>
+      <c r="D21" s="25">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="28">
-        <f>D21+ACTIVE2</f>
+      <c r="E21" s="29"/>
+      <c r="F21" s="25">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="28">
-        <f>F21+ACTIVE3</f>
+      <c r="G21" s="29"/>
+      <c r="H21" s="25">
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="I21" s="32"/>
+      <c r="I21" s="29"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
       <c r="P21"/>
     </row>
     <row r="22" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="27">
         <v>8</v>
       </c>
-      <c r="B22" s="31">
-        <f>H21+ACTIVE4</f>
+      <c r="B22" s="28">
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="28">
-        <f>B22+ACTIVE1</f>
+      <c r="C22" s="29"/>
+      <c r="D22" s="25">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="28">
-        <f>D22+ACTIVE2</f>
+      <c r="E22" s="29"/>
+      <c r="F22" s="25">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="28">
-        <f>F22+ACTIVE3</f>
+      <c r="G22" s="29"/>
+      <c r="H22" s="25">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="I22" s="32"/>
+      <c r="I22" s="29"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="27">
         <v>9</v>
       </c>
-      <c r="B23" s="31">
-        <f>H22+ACTIVE4</f>
+      <c r="B23" s="28">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="28">
-        <f>B23+ACTIVE1</f>
+      <c r="C23" s="29"/>
+      <c r="D23" s="25">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="28">
-        <f>D23+ACTIVE2</f>
+      <c r="E23" s="29"/>
+      <c r="F23" s="25">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="28">
-        <f>F23+ACTIVE3</f>
+      <c r="G23" s="29"/>
+      <c r="H23" s="25">
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="I23" s="32"/>
+      <c r="I23" s="29"/>
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
@@ -2451,1891 +2612,1891 @@
       <c r="S23"/>
     </row>
     <row r="24" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="27">
         <v>10</v>
       </c>
-      <c r="B24" s="31">
-        <f>H23+ACTIVE4</f>
+      <c r="B24" s="28">
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="28">
-        <f>B24+ACTIVE1</f>
+      <c r="C24" s="29"/>
+      <c r="D24" s="25">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="28">
-        <f>D24+ACTIVE2</f>
+      <c r="E24" s="29"/>
+      <c r="F24" s="25">
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="28">
-        <f>F24+ACTIVE3</f>
+      <c r="G24" s="29"/>
+      <c r="H24" s="25">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="I24" s="32"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="A25" s="27">
         <v>11</v>
       </c>
-      <c r="B25" s="31">
-        <f>H24+ACTIVE4</f>
+      <c r="B25" s="28">
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="28">
-        <f>B25+ACTIVE1</f>
+      <c r="C25" s="29"/>
+      <c r="D25" s="25">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="28">
-        <f>D25+ACTIVE2</f>
+      <c r="E25" s="29"/>
+      <c r="F25" s="25">
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="28">
-        <f>F25+ACTIVE3</f>
+      <c r="G25" s="29"/>
+      <c r="H25" s="25">
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="I25" s="32"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="1:19" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33">
+      <c r="A26" s="30">
         <v>12</v>
       </c>
-      <c r="B26" s="34">
-        <f>H25+ACTIVE4</f>
+      <c r="B26" s="31">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="44">
-        <f>B26+ACTIVE1</f>
+      <c r="C26" s="32"/>
+      <c r="D26" s="41">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="44">
-        <f>D26+ACTIVE2</f>
+      <c r="E26" s="32"/>
+      <c r="F26" s="41">
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="G26" s="35"/>
-      <c r="H26" s="44">
-        <f>F26+ACTIVE3</f>
+      <c r="G26" s="32"/>
+      <c r="H26" s="41">
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="32"/>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:19" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H27" s="40" t="s">
+      <c r="H27" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="41">
+      <c r="I27" s="38">
         <f>SUMPRODUCT(LEN(C15:I26)-LEN(SUBSTITUTE(UPPER(C15:I26),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="21"/>
     </row>
     <row r="29" spans="1:19" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="25" t="s">
+      <c r="F29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="I29" s="23" t="s">
         <v>17</v>
       </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:19" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
+      <c r="A30" s="24">
         <v>13</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="25">
         <f>H26+ACTIVE4</f>
         <v>49</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="42">
-        <f>B30+ACTIVE1</f>
+      <c r="C30" s="26"/>
+      <c r="D30" s="39">
+        <f t="shared" ref="D30:D41" si="4">B30+ACTIVE1</f>
         <v>50</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="42">
-        <f>D30+ACTIVE2</f>
+      <c r="E30" s="26"/>
+      <c r="F30" s="39">
+        <f t="shared" ref="F30:F41" si="5">D30+ACTIVE2</f>
         <v>51</v>
       </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="42">
-        <f>F30+ACTIVE3</f>
+      <c r="G30" s="26"/>
+      <c r="H30" s="39">
+        <f t="shared" ref="H30:H41" si="6">F30+ACTIVE3</f>
         <v>52</v>
       </c>
-      <c r="I30" s="29"/>
+      <c r="I30" s="26"/>
     </row>
     <row r="31" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30">
+      <c r="A31" s="27">
         <v>14</v>
       </c>
-      <c r="B31" s="31">
-        <f>H30+ACTIVE4</f>
+      <c r="B31" s="28">
+        <f t="shared" ref="B31:B41" si="7">H30+ACTIVE4</f>
         <v>53</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="28">
-        <f>B31+ACTIVE1</f>
+      <c r="C31" s="29"/>
+      <c r="D31" s="25">
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="28">
-        <f>D31+ACTIVE2</f>
+      <c r="E31" s="29"/>
+      <c r="F31" s="25">
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="28">
-        <f>F31+ACTIVE3</f>
+      <c r="G31" s="29"/>
+      <c r="H31" s="25">
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
-      <c r="I31" s="32"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+      <c r="A32" s="27">
         <v>15</v>
       </c>
-      <c r="B32" s="31">
-        <f>H31+ACTIVE4</f>
+      <c r="B32" s="28">
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="28">
-        <f>B32+ACTIVE1</f>
+      <c r="C32" s="29"/>
+      <c r="D32" s="25">
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="28">
-        <f>D32+ACTIVE2</f>
+      <c r="E32" s="29"/>
+      <c r="F32" s="25">
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="28">
-        <f>F32+ACTIVE3</f>
+      <c r="G32" s="29"/>
+      <c r="H32" s="25">
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="I32" s="32"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30">
+      <c r="A33" s="27">
         <v>16</v>
       </c>
-      <c r="B33" s="31">
-        <f>H32+ACTIVE4</f>
+      <c r="B33" s="28">
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="28">
-        <f>B33+ACTIVE1</f>
+      <c r="C33" s="29"/>
+      <c r="D33" s="25">
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="28">
-        <f>D33+ACTIVE2</f>
+      <c r="E33" s="29"/>
+      <c r="F33" s="25">
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="28">
-        <f>F33+ACTIVE3</f>
+      <c r="G33" s="29"/>
+      <c r="H33" s="25">
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="I33" s="32"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="27">
         <v>17</v>
       </c>
-      <c r="B34" s="31">
-        <f>H33+ACTIVE4</f>
+      <c r="B34" s="28">
+        <f t="shared" si="7"/>
         <v>65</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="28">
-        <f>B34+ACTIVE1</f>
+      <c r="C34" s="29"/>
+      <c r="D34" s="25">
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="28">
-        <f>D34+ACTIVE2</f>
+      <c r="E34" s="29"/>
+      <c r="F34" s="25">
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
-      <c r="G34" s="32"/>
-      <c r="H34" s="28">
-        <f>F34+ACTIVE3</f>
+      <c r="G34" s="29"/>
+      <c r="H34" s="25">
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
-      <c r="I34" s="32"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30">
+      <c r="A35" s="27">
         <v>18</v>
       </c>
-      <c r="B35" s="31">
-        <f>H34+ACTIVE4</f>
+      <c r="B35" s="28">
+        <f t="shared" si="7"/>
         <v>69</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="28">
-        <f>B35+ACTIVE1</f>
+      <c r="C35" s="29"/>
+      <c r="D35" s="25">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="28">
-        <f>D35+ACTIVE2</f>
+      <c r="E35" s="29"/>
+      <c r="F35" s="25">
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="28">
-        <f>F35+ACTIVE3</f>
+      <c r="G35" s="29"/>
+      <c r="H35" s="25">
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
-      <c r="I35" s="32"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="36" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30">
+      <c r="A36" s="27">
         <v>19</v>
       </c>
-      <c r="B36" s="31">
-        <f>H35+ACTIVE4</f>
+      <c r="B36" s="28">
+        <f t="shared" si="7"/>
         <v>73</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="28">
-        <f>B36+ACTIVE1</f>
+      <c r="C36" s="29"/>
+      <c r="D36" s="25">
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="28">
-        <f>D36+ACTIVE2</f>
+      <c r="E36" s="29"/>
+      <c r="F36" s="25">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
-      <c r="G36" s="32"/>
-      <c r="H36" s="28">
-        <f>F36+ACTIVE3</f>
+      <c r="G36" s="29"/>
+      <c r="H36" s="25">
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
-      <c r="I36" s="32"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30">
+      <c r="A37" s="27">
         <v>20</v>
       </c>
-      <c r="B37" s="31">
-        <f>H36+ACTIVE4</f>
+      <c r="B37" s="28">
+        <f t="shared" si="7"/>
         <v>77</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="28">
-        <f>B37+ACTIVE1</f>
+      <c r="C37" s="29"/>
+      <c r="D37" s="25">
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="28">
-        <f>D37+ACTIVE2</f>
+      <c r="E37" s="29"/>
+      <c r="F37" s="25">
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
-      <c r="G37" s="32"/>
-      <c r="H37" s="28">
-        <f>F37+ACTIVE3</f>
+      <c r="G37" s="29"/>
+      <c r="H37" s="25">
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
-      <c r="I37" s="32"/>
+      <c r="I37" s="29"/>
     </row>
     <row r="38" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30">
+      <c r="A38" s="27">
         <v>21</v>
       </c>
-      <c r="B38" s="31">
-        <f>H37+ACTIVE4</f>
+      <c r="B38" s="28">
+        <f t="shared" si="7"/>
         <v>81</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="28">
-        <f>B38+ACTIVE1</f>
+      <c r="C38" s="29"/>
+      <c r="D38" s="25">
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="28">
-        <f>D38+ACTIVE2</f>
+      <c r="E38" s="29"/>
+      <c r="F38" s="25">
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
-      <c r="G38" s="32"/>
-      <c r="H38" s="28">
-        <f>F38+ACTIVE3</f>
+      <c r="G38" s="29"/>
+      <c r="H38" s="25">
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
-      <c r="I38" s="32"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30">
+      <c r="A39" s="27">
         <v>22</v>
       </c>
-      <c r="B39" s="31">
-        <f>H38+ACTIVE4</f>
+      <c r="B39" s="28">
+        <f t="shared" si="7"/>
         <v>85</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="28">
-        <f>B39+ACTIVE1</f>
+      <c r="C39" s="29"/>
+      <c r="D39" s="25">
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="28">
-        <f>D39+ACTIVE2</f>
+      <c r="E39" s="29"/>
+      <c r="F39" s="25">
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
-      <c r="G39" s="32"/>
-      <c r="H39" s="28">
-        <f>F39+ACTIVE3</f>
+      <c r="G39" s="29"/>
+      <c r="H39" s="25">
+        <f t="shared" si="6"/>
         <v>88</v>
       </c>
-      <c r="I39" s="32"/>
+      <c r="I39" s="29"/>
     </row>
     <row r="40" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30">
+      <c r="A40" s="27">
         <v>23</v>
       </c>
-      <c r="B40" s="31">
-        <f>H39+ACTIVE4</f>
+      <c r="B40" s="28">
+        <f t="shared" si="7"/>
         <v>89</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="28">
-        <f>B40+ACTIVE1</f>
+      <c r="C40" s="29"/>
+      <c r="D40" s="25">
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="28">
-        <f>D40+ACTIVE2</f>
+      <c r="E40" s="29"/>
+      <c r="F40" s="25">
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
-      <c r="G40" s="32"/>
-      <c r="H40" s="28">
-        <f>F40+ACTIVE3</f>
+      <c r="G40" s="29"/>
+      <c r="H40" s="25">
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
-      <c r="I40" s="32"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="33">
+      <c r="A41" s="30">
         <v>24</v>
       </c>
-      <c r="B41" s="34">
-        <f>H40+ACTIVE4</f>
+      <c r="B41" s="31">
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="44">
-        <f>B41+ACTIVE1</f>
+      <c r="C41" s="32"/>
+      <c r="D41" s="41">
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="44">
-        <f>D41+ACTIVE2</f>
+      <c r="E41" s="32"/>
+      <c r="F41" s="41">
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
-      <c r="G41" s="35"/>
-      <c r="H41" s="44">
-        <f>F41+ACTIVE3</f>
+      <c r="G41" s="32"/>
+      <c r="H41" s="41">
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
-      <c r="I41" s="35"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H42" s="40" t="s">
+      <c r="H42" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="41">
+      <c r="I42" s="38">
         <f>SUMPRODUCT(LEN(C30:I41)-LEN(SUBSTITUTE(UPPER(C30:I41),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="21"/>
     </row>
     <row r="44" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D44" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E44" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="25" t="s">
+      <c r="F44" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G44" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="25" t="s">
+      <c r="H44" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="26" t="s">
+      <c r="I44" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27">
+      <c r="A45" s="24">
         <v>25</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="25">
         <f>H41+ACTIVE4</f>
         <v>97</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="42">
-        <f>B45+ACTIVE1</f>
+      <c r="C45" s="26"/>
+      <c r="D45" s="39">
+        <f t="shared" ref="D45:D56" si="8">B45+ACTIVE1</f>
         <v>98</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="42">
-        <f>D45+ACTIVE2</f>
+      <c r="E45" s="26"/>
+      <c r="F45" s="39">
+        <f t="shared" ref="F45:F56" si="9">D45+ACTIVE2</f>
         <v>99</v>
       </c>
-      <c r="G45" s="29"/>
-      <c r="H45" s="42">
-        <f>F45+ACTIVE3</f>
+      <c r="G45" s="26"/>
+      <c r="H45" s="39">
+        <f t="shared" ref="H45:H56" si="10">F45+ACTIVE3</f>
         <v>100</v>
       </c>
-      <c r="I45" s="29"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30">
+      <c r="A46" s="27">
         <v>26</v>
       </c>
-      <c r="B46" s="31">
-        <f>H45+ACTIVE4</f>
+      <c r="B46" s="28">
+        <f t="shared" ref="B46:B56" si="11">H45+ACTIVE4</f>
         <v>101</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="28">
-        <f>B46+ACTIVE1</f>
+      <c r="C46" s="29"/>
+      <c r="D46" s="25">
+        <f t="shared" si="8"/>
         <v>102</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="28">
-        <f>D46+ACTIVE2</f>
+      <c r="E46" s="29"/>
+      <c r="F46" s="25">
+        <f t="shared" si="9"/>
         <v>103</v>
       </c>
-      <c r="G46" s="32"/>
-      <c r="H46" s="28">
-        <f>F46+ACTIVE3</f>
+      <c r="G46" s="29"/>
+      <c r="H46" s="25">
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
-      <c r="I46" s="32"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="30">
+      <c r="A47" s="27">
         <v>27</v>
       </c>
-      <c r="B47" s="31">
-        <f>H46+ACTIVE4</f>
+      <c r="B47" s="28">
+        <f t="shared" si="11"/>
         <v>105</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="28">
-        <f>B47+ACTIVE1</f>
+      <c r="C47" s="29"/>
+      <c r="D47" s="25">
+        <f t="shared" si="8"/>
         <v>106</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="28">
-        <f>D47+ACTIVE2</f>
+      <c r="E47" s="29"/>
+      <c r="F47" s="25">
+        <f t="shared" si="9"/>
         <v>107</v>
       </c>
-      <c r="G47" s="32"/>
-      <c r="H47" s="28">
-        <f>F47+ACTIVE3</f>
+      <c r="G47" s="29"/>
+      <c r="H47" s="25">
+        <f t="shared" si="10"/>
         <v>108</v>
       </c>
-      <c r="I47" s="32"/>
+      <c r="I47" s="29"/>
     </row>
     <row r="48" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30">
+      <c r="A48" s="27">
         <v>28</v>
       </c>
-      <c r="B48" s="31">
-        <f>H47+ACTIVE4</f>
+      <c r="B48" s="28">
+        <f t="shared" si="11"/>
         <v>109</v>
       </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="28">
-        <f>B48+ACTIVE1</f>
+      <c r="C48" s="29"/>
+      <c r="D48" s="25">
+        <f t="shared" si="8"/>
         <v>110</v>
       </c>
-      <c r="E48" s="32"/>
-      <c r="F48" s="28">
-        <f>D48+ACTIVE2</f>
+      <c r="E48" s="29"/>
+      <c r="F48" s="25">
+        <f t="shared" si="9"/>
         <v>111</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="28">
-        <f>F48+ACTIVE3</f>
+      <c r="G48" s="29"/>
+      <c r="H48" s="25">
+        <f t="shared" si="10"/>
         <v>112</v>
       </c>
-      <c r="I48" s="32"/>
+      <c r="I48" s="29"/>
     </row>
     <row r="49" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30">
+      <c r="A49" s="27">
         <v>29</v>
       </c>
-      <c r="B49" s="31">
-        <f>H48+ACTIVE4</f>
+      <c r="B49" s="28">
+        <f t="shared" si="11"/>
         <v>113</v>
       </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="28">
-        <f>B49+ACTIVE1</f>
+      <c r="C49" s="29"/>
+      <c r="D49" s="25">
+        <f t="shared" si="8"/>
         <v>114</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="28">
-        <f>D49+ACTIVE2</f>
+      <c r="E49" s="29"/>
+      <c r="F49" s="25">
+        <f t="shared" si="9"/>
         <v>115</v>
       </c>
-      <c r="G49" s="32"/>
-      <c r="H49" s="28">
-        <f>F49+ACTIVE3</f>
+      <c r="G49" s="29"/>
+      <c r="H49" s="25">
+        <f t="shared" si="10"/>
         <v>116</v>
       </c>
-      <c r="I49" s="32"/>
+      <c r="I49" s="29"/>
     </row>
     <row r="50" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30">
+      <c r="A50" s="27">
         <v>30</v>
       </c>
-      <c r="B50" s="31">
-        <f>H49+ACTIVE4</f>
+      <c r="B50" s="28">
+        <f t="shared" si="11"/>
         <v>117</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="28">
-        <f>B50+ACTIVE1</f>
+      <c r="C50" s="29"/>
+      <c r="D50" s="25">
+        <f t="shared" si="8"/>
         <v>118</v>
       </c>
-      <c r="E50" s="32"/>
-      <c r="F50" s="28">
-        <f>D50+ACTIVE2</f>
+      <c r="E50" s="29"/>
+      <c r="F50" s="25">
+        <f t="shared" si="9"/>
         <v>119</v>
       </c>
-      <c r="G50" s="32"/>
-      <c r="H50" s="28">
-        <f>F50+ACTIVE3</f>
+      <c r="G50" s="29"/>
+      <c r="H50" s="25">
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="I50" s="32"/>
+      <c r="I50" s="29"/>
     </row>
     <row r="51" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30">
+      <c r="A51" s="27">
         <v>31</v>
       </c>
-      <c r="B51" s="31">
-        <f>H50+ACTIVE4</f>
+      <c r="B51" s="28">
+        <f t="shared" si="11"/>
         <v>121</v>
       </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="28">
-        <f>B51+ACTIVE1</f>
+      <c r="C51" s="29"/>
+      <c r="D51" s="25">
+        <f t="shared" si="8"/>
         <v>122</v>
       </c>
-      <c r="E51" s="32"/>
-      <c r="F51" s="28">
-        <f>D51+ACTIVE2</f>
+      <c r="E51" s="29"/>
+      <c r="F51" s="25">
+        <f t="shared" si="9"/>
         <v>123</v>
       </c>
-      <c r="G51" s="32"/>
-      <c r="H51" s="28">
-        <f>F51+ACTIVE3</f>
+      <c r="G51" s="29"/>
+      <c r="H51" s="25">
+        <f t="shared" si="10"/>
         <v>124</v>
       </c>
-      <c r="I51" s="32"/>
+      <c r="I51" s="29"/>
     </row>
     <row r="52" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="30">
+      <c r="A52" s="27">
         <v>32</v>
       </c>
-      <c r="B52" s="31">
-        <f>H51+ACTIVE4</f>
+      <c r="B52" s="28">
+        <f t="shared" si="11"/>
         <v>125</v>
       </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="28">
-        <f>B52+ACTIVE1</f>
+      <c r="C52" s="29"/>
+      <c r="D52" s="25">
+        <f t="shared" si="8"/>
         <v>126</v>
       </c>
-      <c r="E52" s="32"/>
-      <c r="F52" s="28">
-        <f>D52+ACTIVE2</f>
+      <c r="E52" s="29"/>
+      <c r="F52" s="25">
+        <f t="shared" si="9"/>
         <v>127</v>
       </c>
-      <c r="G52" s="32"/>
-      <c r="H52" s="28">
-        <f>F52+ACTIVE3</f>
+      <c r="G52" s="29"/>
+      <c r="H52" s="25">
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
-      <c r="I52" s="32"/>
+      <c r="I52" s="29"/>
     </row>
     <row r="53" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30">
+      <c r="A53" s="27">
         <v>33</v>
       </c>
-      <c r="B53" s="31">
-        <f>H52+ACTIVE4</f>
+      <c r="B53" s="28">
+        <f t="shared" si="11"/>
         <v>129</v>
       </c>
-      <c r="C53" s="32"/>
-      <c r="D53" s="28">
-        <f>B53+ACTIVE1</f>
+      <c r="C53" s="29"/>
+      <c r="D53" s="25">
+        <f t="shared" si="8"/>
         <v>130</v>
       </c>
-      <c r="E53" s="32"/>
-      <c r="F53" s="28">
-        <f>D53+ACTIVE2</f>
+      <c r="E53" s="29"/>
+      <c r="F53" s="25">
+        <f t="shared" si="9"/>
         <v>131</v>
       </c>
-      <c r="G53" s="32"/>
-      <c r="H53" s="28">
-        <f>F53+ACTIVE3</f>
+      <c r="G53" s="29"/>
+      <c r="H53" s="25">
+        <f t="shared" si="10"/>
         <v>132</v>
       </c>
-      <c r="I53" s="32"/>
+      <c r="I53" s="29"/>
     </row>
     <row r="54" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="30">
+      <c r="A54" s="27">
         <v>34</v>
       </c>
-      <c r="B54" s="31">
-        <f>H53+ACTIVE4</f>
+      <c r="B54" s="28">
+        <f t="shared" si="11"/>
         <v>133</v>
       </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="28">
-        <f>B54+ACTIVE1</f>
+      <c r="C54" s="29"/>
+      <c r="D54" s="25">
+        <f t="shared" si="8"/>
         <v>134</v>
       </c>
-      <c r="E54" s="32"/>
-      <c r="F54" s="28">
-        <f>D54+ACTIVE2</f>
+      <c r="E54" s="29"/>
+      <c r="F54" s="25">
+        <f t="shared" si="9"/>
         <v>135</v>
       </c>
-      <c r="G54" s="32"/>
-      <c r="H54" s="28">
-        <f>F54+ACTIVE3</f>
+      <c r="G54" s="29"/>
+      <c r="H54" s="25">
+        <f t="shared" si="10"/>
         <v>136</v>
       </c>
-      <c r="I54" s="32"/>
+      <c r="I54" s="29"/>
     </row>
     <row r="55" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30">
+      <c r="A55" s="27">
         <v>35</v>
       </c>
-      <c r="B55" s="31">
-        <f>H54+ACTIVE4</f>
+      <c r="B55" s="28">
+        <f t="shared" si="11"/>
         <v>137</v>
       </c>
-      <c r="C55" s="32"/>
-      <c r="D55" s="28">
-        <f>B55+ACTIVE1</f>
+      <c r="C55" s="29"/>
+      <c r="D55" s="25">
+        <f t="shared" si="8"/>
         <v>138</v>
       </c>
-      <c r="E55" s="32"/>
-      <c r="F55" s="28">
-        <f>D55+ACTIVE2</f>
+      <c r="E55" s="29"/>
+      <c r="F55" s="25">
+        <f t="shared" si="9"/>
         <v>139</v>
       </c>
-      <c r="G55" s="32"/>
-      <c r="H55" s="28">
-        <f>F55+ACTIVE3</f>
+      <c r="G55" s="29"/>
+      <c r="H55" s="25">
+        <f t="shared" si="10"/>
         <v>140</v>
       </c>
-      <c r="I55" s="32"/>
+      <c r="I55" s="29"/>
     </row>
     <row r="56" spans="1:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="33">
+      <c r="A56" s="30">
         <v>36</v>
       </c>
-      <c r="B56" s="34">
-        <f>H55+ACTIVE4</f>
+      <c r="B56" s="31">
+        <f t="shared" si="11"/>
         <v>141</v>
       </c>
-      <c r="C56" s="35"/>
-      <c r="D56" s="44">
-        <f>B56+ACTIVE1</f>
+      <c r="C56" s="32"/>
+      <c r="D56" s="41">
+        <f t="shared" si="8"/>
         <v>142</v>
       </c>
-      <c r="E56" s="35"/>
-      <c r="F56" s="44">
-        <f>D56+ACTIVE2</f>
+      <c r="E56" s="32"/>
+      <c r="F56" s="41">
+        <f t="shared" si="9"/>
         <v>143</v>
       </c>
-      <c r="G56" s="35"/>
-      <c r="H56" s="44">
-        <f>F56+ACTIVE3</f>
+      <c r="G56" s="32"/>
+      <c r="H56" s="41">
+        <f t="shared" si="10"/>
         <v>144</v>
       </c>
-      <c r="I56" s="35"/>
+      <c r="I56" s="32"/>
     </row>
     <row r="57" spans="1:12" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H57" s="36" t="s">
+      <c r="H57" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I57" s="37">
+      <c r="I57" s="34">
         <f>SUMPRODUCT(LEN(C45:I56)-LEN(SUBSTITUTE(UPPER(C45:I56),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="24"/>
+      <c r="C58" s="21"/>
     </row>
     <row r="59" spans="1:12" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E59" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F59" s="25" t="s">
+      <c r="F59" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G59" s="26" t="s">
+      <c r="G59" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="25" t="s">
+      <c r="H59" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I59" s="26" t="s">
+      <c r="I59" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="38">
+      <c r="A60" s="35">
         <v>37</v>
       </c>
-      <c r="B60" s="28">
+      <c r="B60" s="25">
         <f>H56+ACTIVE4</f>
         <v>145</v>
       </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="42">
-        <f>B60+ACTIVE1</f>
+      <c r="C60" s="26"/>
+      <c r="D60" s="39">
+        <f t="shared" ref="D60:D71" si="12">B60+ACTIVE1</f>
         <v>146</v>
       </c>
-      <c r="E60" s="29"/>
-      <c r="F60" s="42">
-        <f>D60+ACTIVE2</f>
+      <c r="E60" s="26"/>
+      <c r="F60" s="39">
+        <f t="shared" ref="F60:F71" si="13">D60+ACTIVE2</f>
         <v>147</v>
       </c>
-      <c r="G60" s="29"/>
-      <c r="H60" s="42">
-        <f>F60+ACTIVE3</f>
+      <c r="G60" s="26"/>
+      <c r="H60" s="39">
+        <f t="shared" ref="H60:H71" si="14">F60+ACTIVE3</f>
         <v>148</v>
       </c>
-      <c r="I60" s="29"/>
+      <c r="I60" s="26"/>
     </row>
     <row r="61" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="30">
+      <c r="A61" s="27">
         <v>38</v>
       </c>
-      <c r="B61" s="31">
-        <f>H60+ACTIVE4</f>
+      <c r="B61" s="28">
+        <f t="shared" ref="B61:B71" si="15">H60+ACTIVE4</f>
         <v>149</v>
       </c>
-      <c r="C61" s="32"/>
-      <c r="D61" s="28">
-        <f>B61+ACTIVE1</f>
+      <c r="C61" s="29"/>
+      <c r="D61" s="25">
+        <f t="shared" si="12"/>
         <v>150</v>
       </c>
-      <c r="E61" s="32"/>
-      <c r="F61" s="28">
-        <f>D61+ACTIVE2</f>
+      <c r="E61" s="29"/>
+      <c r="F61" s="25">
+        <f t="shared" si="13"/>
         <v>151</v>
       </c>
-      <c r="G61" s="32"/>
-      <c r="H61" s="28">
-        <f>F61+ACTIVE3</f>
+      <c r="G61" s="29"/>
+      <c r="H61" s="25">
+        <f t="shared" si="14"/>
         <v>152</v>
       </c>
-      <c r="I61" s="32"/>
-      <c r="L61" s="4" t="s">
+      <c r="I61" s="29"/>
+      <c r="L61" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="27">
+      <c r="A62" s="24">
         <v>39</v>
       </c>
-      <c r="B62" s="31">
-        <f>H61+ACTIVE4</f>
+      <c r="B62" s="28">
+        <f t="shared" si="15"/>
         <v>153</v>
       </c>
-      <c r="C62" s="32"/>
-      <c r="D62" s="28">
-        <f>B62+ACTIVE1</f>
+      <c r="C62" s="29"/>
+      <c r="D62" s="25">
+        <f t="shared" si="12"/>
         <v>154</v>
       </c>
-      <c r="E62" s="32"/>
-      <c r="F62" s="28">
-        <f>D62+ACTIVE2</f>
+      <c r="E62" s="29"/>
+      <c r="F62" s="25">
+        <f t="shared" si="13"/>
         <v>155</v>
       </c>
-      <c r="G62" s="32"/>
-      <c r="H62" s="28">
-        <f>F62+ACTIVE3</f>
+      <c r="G62" s="29"/>
+      <c r="H62" s="25">
+        <f t="shared" si="14"/>
         <v>156</v>
       </c>
-      <c r="I62" s="32"/>
+      <c r="I62" s="29"/>
     </row>
     <row r="63" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="30">
+      <c r="A63" s="27">
         <v>40</v>
       </c>
-      <c r="B63" s="31">
-        <f>H62+ACTIVE4</f>
+      <c r="B63" s="28">
+        <f t="shared" si="15"/>
         <v>157</v>
       </c>
-      <c r="C63" s="32"/>
-      <c r="D63" s="28">
-        <f>B63+ACTIVE1</f>
+      <c r="C63" s="29"/>
+      <c r="D63" s="25">
+        <f t="shared" si="12"/>
         <v>158</v>
       </c>
-      <c r="E63" s="32"/>
-      <c r="F63" s="28">
-        <f>D63+ACTIVE2</f>
+      <c r="E63" s="29"/>
+      <c r="F63" s="25">
+        <f t="shared" si="13"/>
         <v>159</v>
       </c>
-      <c r="G63" s="32"/>
-      <c r="H63" s="28">
-        <f>F63+ACTIVE3</f>
+      <c r="G63" s="29"/>
+      <c r="H63" s="25">
+        <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="I63" s="32"/>
+      <c r="I63" s="29"/>
     </row>
     <row r="64" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="27">
+      <c r="A64" s="24">
         <v>41</v>
       </c>
-      <c r="B64" s="31">
-        <f>H63+ACTIVE4</f>
+      <c r="B64" s="28">
+        <f t="shared" si="15"/>
         <v>161</v>
       </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="28">
-        <f>B64+ACTIVE1</f>
+      <c r="C64" s="29"/>
+      <c r="D64" s="25">
+        <f t="shared" si="12"/>
         <v>162</v>
       </c>
-      <c r="E64" s="32"/>
-      <c r="F64" s="28">
-        <f>D64+ACTIVE2</f>
+      <c r="E64" s="29"/>
+      <c r="F64" s="25">
+        <f t="shared" si="13"/>
         <v>163</v>
       </c>
-      <c r="G64" s="32"/>
-      <c r="H64" s="28">
-        <f>F64+ACTIVE3</f>
+      <c r="G64" s="29"/>
+      <c r="H64" s="25">
+        <f t="shared" si="14"/>
         <v>164</v>
       </c>
-      <c r="I64" s="32"/>
+      <c r="I64" s="29"/>
     </row>
     <row r="65" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30">
+      <c r="A65" s="27">
         <v>42</v>
       </c>
-      <c r="B65" s="31">
-        <f>H64+ACTIVE4</f>
+      <c r="B65" s="28">
+        <f t="shared" si="15"/>
         <v>165</v>
       </c>
-      <c r="C65" s="32"/>
-      <c r="D65" s="28">
-        <f>B65+ACTIVE1</f>
+      <c r="C65" s="29"/>
+      <c r="D65" s="25">
+        <f t="shared" si="12"/>
         <v>166</v>
       </c>
-      <c r="E65" s="32"/>
-      <c r="F65" s="28">
-        <f>D65+ACTIVE2</f>
+      <c r="E65" s="29"/>
+      <c r="F65" s="25">
+        <f t="shared" si="13"/>
         <v>167</v>
       </c>
-      <c r="G65" s="32"/>
-      <c r="H65" s="28">
-        <f>F65+ACTIVE3</f>
+      <c r="G65" s="29"/>
+      <c r="H65" s="25">
+        <f t="shared" si="14"/>
         <v>168</v>
       </c>
-      <c r="I65" s="32"/>
+      <c r="I65" s="29"/>
     </row>
     <row r="66" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="27">
+      <c r="A66" s="24">
         <v>43</v>
       </c>
-      <c r="B66" s="31">
-        <f>H65+ACTIVE4</f>
+      <c r="B66" s="28">
+        <f t="shared" si="15"/>
         <v>169</v>
       </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="28">
-        <f>B66+ACTIVE1</f>
+      <c r="C66" s="29"/>
+      <c r="D66" s="25">
+        <f t="shared" si="12"/>
         <v>170</v>
       </c>
-      <c r="E66" s="32"/>
-      <c r="F66" s="28">
-        <f>D66+ACTIVE2</f>
+      <c r="E66" s="29"/>
+      <c r="F66" s="25">
+        <f t="shared" si="13"/>
         <v>171</v>
       </c>
-      <c r="G66" s="32"/>
-      <c r="H66" s="28">
-        <f>F66+ACTIVE3</f>
+      <c r="G66" s="29"/>
+      <c r="H66" s="25">
+        <f t="shared" si="14"/>
         <v>172</v>
       </c>
-      <c r="I66" s="32"/>
+      <c r="I66" s="29"/>
     </row>
     <row r="67" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30">
+      <c r="A67" s="27">
         <v>44</v>
       </c>
-      <c r="B67" s="31">
-        <f>H66+ACTIVE4</f>
+      <c r="B67" s="28">
+        <f t="shared" si="15"/>
         <v>173</v>
       </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="28">
-        <f>B67+ACTIVE1</f>
+      <c r="C67" s="29"/>
+      <c r="D67" s="25">
+        <f t="shared" si="12"/>
         <v>174</v>
       </c>
-      <c r="E67" s="32"/>
-      <c r="F67" s="28">
-        <f>D67+ACTIVE2</f>
+      <c r="E67" s="29"/>
+      <c r="F67" s="25">
+        <f t="shared" si="13"/>
         <v>175</v>
       </c>
-      <c r="G67" s="32"/>
-      <c r="H67" s="28">
-        <f>F67+ACTIVE3</f>
+      <c r="G67" s="29"/>
+      <c r="H67" s="25">
+        <f t="shared" si="14"/>
         <v>176</v>
       </c>
-      <c r="I67" s="32"/>
+      <c r="I67" s="29"/>
     </row>
     <row r="68" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="27">
+      <c r="A68" s="24">
         <v>45</v>
       </c>
-      <c r="B68" s="31">
-        <f>H67+ACTIVE4</f>
+      <c r="B68" s="28">
+        <f t="shared" si="15"/>
         <v>177</v>
       </c>
-      <c r="C68" s="32"/>
-      <c r="D68" s="28">
-        <f>B68+ACTIVE1</f>
+      <c r="C68" s="29"/>
+      <c r="D68" s="25">
+        <f t="shared" si="12"/>
         <v>178</v>
       </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="28">
-        <f>D68+ACTIVE2</f>
+      <c r="E68" s="29"/>
+      <c r="F68" s="25">
+        <f t="shared" si="13"/>
         <v>179</v>
       </c>
-      <c r="G68" s="32"/>
-      <c r="H68" s="28">
-        <f>F68+ACTIVE3</f>
+      <c r="G68" s="29"/>
+      <c r="H68" s="25">
+        <f t="shared" si="14"/>
         <v>180</v>
       </c>
-      <c r="I68" s="32"/>
+      <c r="I68" s="29"/>
     </row>
     <row r="69" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30">
+      <c r="A69" s="27">
         <v>46</v>
       </c>
-      <c r="B69" s="31">
-        <f>H68+ACTIVE4</f>
+      <c r="B69" s="28">
+        <f t="shared" si="15"/>
         <v>181</v>
       </c>
-      <c r="C69" s="32"/>
-      <c r="D69" s="28">
-        <f>B69+ACTIVE1</f>
+      <c r="C69" s="29"/>
+      <c r="D69" s="25">
+        <f t="shared" si="12"/>
         <v>182</v>
       </c>
-      <c r="E69" s="32"/>
-      <c r="F69" s="28">
-        <f>D69+ACTIVE2</f>
+      <c r="E69" s="29"/>
+      <c r="F69" s="25">
+        <f t="shared" si="13"/>
         <v>183</v>
       </c>
-      <c r="G69" s="32"/>
-      <c r="H69" s="28">
-        <f>F69+ACTIVE3</f>
+      <c r="G69" s="29"/>
+      <c r="H69" s="25">
+        <f t="shared" si="14"/>
         <v>184</v>
       </c>
-      <c r="I69" s="32"/>
+      <c r="I69" s="29"/>
     </row>
     <row r="70" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="27">
+      <c r="A70" s="24">
         <v>47</v>
       </c>
-      <c r="B70" s="31">
-        <f>H69+ACTIVE4</f>
+      <c r="B70" s="28">
+        <f t="shared" si="15"/>
         <v>185</v>
       </c>
-      <c r="C70" s="32"/>
-      <c r="D70" s="28">
-        <f>B70+ACTIVE1</f>
+      <c r="C70" s="29"/>
+      <c r="D70" s="25">
+        <f t="shared" si="12"/>
         <v>186</v>
       </c>
-      <c r="E70" s="32"/>
-      <c r="F70" s="28">
-        <f>D70+ACTIVE2</f>
+      <c r="E70" s="29"/>
+      <c r="F70" s="25">
+        <f t="shared" si="13"/>
         <v>187</v>
       </c>
-      <c r="G70" s="32"/>
-      <c r="H70" s="28">
-        <f>F70+ACTIVE3</f>
+      <c r="G70" s="29"/>
+      <c r="H70" s="25">
+        <f t="shared" si="14"/>
         <v>188</v>
       </c>
-      <c r="I70" s="32"/>
+      <c r="I70" s="29"/>
     </row>
     <row r="71" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="33">
+      <c r="A71" s="30">
         <v>48</v>
       </c>
-      <c r="B71" s="34">
-        <f>H70+ACTIVE4</f>
+      <c r="B71" s="31">
+        <f t="shared" si="15"/>
         <v>189</v>
       </c>
-      <c r="C71" s="35"/>
-      <c r="D71" s="44">
-        <f>B71+ACTIVE1</f>
+      <c r="C71" s="32"/>
+      <c r="D71" s="41">
+        <f t="shared" si="12"/>
         <v>190</v>
       </c>
-      <c r="E71" s="35"/>
-      <c r="F71" s="44">
-        <f>D71+ACTIVE2</f>
+      <c r="E71" s="32"/>
+      <c r="F71" s="41">
+        <f t="shared" si="13"/>
         <v>191</v>
       </c>
-      <c r="G71" s="35"/>
-      <c r="H71" s="44">
-        <f>F71+ACTIVE3</f>
+      <c r="G71" s="32"/>
+      <c r="H71" s="41">
+        <f t="shared" si="14"/>
         <v>192</v>
       </c>
-      <c r="I71" s="35"/>
+      <c r="I71" s="32"/>
     </row>
     <row r="72" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H72" s="36" t="s">
+      <c r="H72" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I72" s="37">
+      <c r="I72" s="34">
         <f>SUMPRODUCT(LEN(C60:I71)-LEN(SUBSTITUTE(UPPER(C60:I71),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="24"/>
+      <c r="C73" s="21"/>
     </row>
     <row r="74" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="18" t="s">
+      <c r="A74" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="B74" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="25" t="s">
+      <c r="D74" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E74" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F74" s="25" t="s">
+      <c r="F74" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G74" s="26" t="s">
+      <c r="G74" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H74" s="25" t="s">
+      <c r="H74" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I74" s="26" t="s">
+      <c r="I74" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="38">
+      <c r="A75" s="35">
         <v>49</v>
       </c>
-      <c r="B75" s="28">
+      <c r="B75" s="25">
         <f>H71+ACTIVE4</f>
         <v>193</v>
       </c>
-      <c r="C75" s="29"/>
-      <c r="D75" s="42">
-        <f>B75+ACTIVE1</f>
+      <c r="C75" s="26"/>
+      <c r="D75" s="39">
+        <f t="shared" ref="D75:D86" si="16">B75+ACTIVE1</f>
         <v>194</v>
       </c>
-      <c r="E75" s="29"/>
-      <c r="F75" s="42">
-        <f>D75+ACTIVE2</f>
+      <c r="E75" s="26"/>
+      <c r="F75" s="39">
+        <f t="shared" ref="F75:F86" si="17">D75+ACTIVE2</f>
         <v>195</v>
       </c>
-      <c r="G75" s="29"/>
-      <c r="H75" s="42">
-        <f>F75+ACTIVE3</f>
+      <c r="G75" s="26"/>
+      <c r="H75" s="39">
+        <f t="shared" ref="H75:H86" si="18">F75+ACTIVE3</f>
         <v>196</v>
       </c>
-      <c r="I75" s="29"/>
+      <c r="I75" s="26"/>
     </row>
     <row r="76" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30">
+      <c r="A76" s="27">
         <v>50</v>
       </c>
-      <c r="B76" s="31">
-        <f>H75+ACTIVE4</f>
+      <c r="B76" s="28">
+        <f t="shared" ref="B76:B86" si="19">H75+ACTIVE4</f>
         <v>197</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="28">
-        <f>B76+ACTIVE1</f>
+      <c r="C76" s="29"/>
+      <c r="D76" s="25">
+        <f t="shared" si="16"/>
         <v>198</v>
       </c>
-      <c r="E76" s="32"/>
-      <c r="F76" s="28">
-        <f>D76+ACTIVE2</f>
+      <c r="E76" s="29"/>
+      <c r="F76" s="25">
+        <f t="shared" si="17"/>
         <v>199</v>
       </c>
-      <c r="G76" s="32"/>
-      <c r="H76" s="28">
-        <f>F76+ACTIVE3</f>
+      <c r="G76" s="29"/>
+      <c r="H76" s="25">
+        <f t="shared" si="18"/>
         <v>200</v>
       </c>
-      <c r="I76" s="32"/>
+      <c r="I76" s="29"/>
     </row>
     <row r="77" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="27">
+      <c r="A77" s="24">
         <v>51</v>
       </c>
-      <c r="B77" s="31">
-        <f>H76+ACTIVE4</f>
+      <c r="B77" s="28">
+        <f t="shared" si="19"/>
         <v>201</v>
       </c>
-      <c r="C77" s="32"/>
-      <c r="D77" s="28">
-        <f>B77+ACTIVE1</f>
+      <c r="C77" s="29"/>
+      <c r="D77" s="25">
+        <f t="shared" si="16"/>
         <v>202</v>
       </c>
-      <c r="E77" s="32"/>
-      <c r="F77" s="28">
-        <f>D77+ACTIVE2</f>
+      <c r="E77" s="29"/>
+      <c r="F77" s="25">
+        <f t="shared" si="17"/>
         <v>203</v>
       </c>
-      <c r="G77" s="32"/>
-      <c r="H77" s="28">
-        <f>F77+ACTIVE3</f>
+      <c r="G77" s="29"/>
+      <c r="H77" s="25">
+        <f t="shared" si="18"/>
         <v>204</v>
       </c>
-      <c r="I77" s="32"/>
+      <c r="I77" s="29"/>
     </row>
     <row r="78" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="30">
+      <c r="A78" s="27">
         <v>52</v>
       </c>
-      <c r="B78" s="31">
-        <f>H77+ACTIVE4</f>
+      <c r="B78" s="28">
+        <f t="shared" si="19"/>
         <v>205</v>
       </c>
-      <c r="C78" s="32"/>
-      <c r="D78" s="28">
-        <f>B78+ACTIVE1</f>
+      <c r="C78" s="29"/>
+      <c r="D78" s="25">
+        <f t="shared" si="16"/>
         <v>206</v>
       </c>
-      <c r="E78" s="32"/>
-      <c r="F78" s="28">
-        <f>D78+ACTIVE2</f>
+      <c r="E78" s="29"/>
+      <c r="F78" s="25">
+        <f t="shared" si="17"/>
         <v>207</v>
       </c>
-      <c r="G78" s="32"/>
-      <c r="H78" s="28">
-        <f>F78+ACTIVE3</f>
+      <c r="G78" s="29"/>
+      <c r="H78" s="25">
+        <f t="shared" si="18"/>
         <v>208</v>
       </c>
-      <c r="I78" s="32"/>
+      <c r="I78" s="29"/>
     </row>
     <row r="79" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="27">
+      <c r="A79" s="24">
         <v>53</v>
       </c>
-      <c r="B79" s="31">
-        <f>H78+ACTIVE4</f>
+      <c r="B79" s="28">
+        <f t="shared" si="19"/>
         <v>209</v>
       </c>
-      <c r="C79" s="32"/>
-      <c r="D79" s="28">
-        <f>B79+ACTIVE1</f>
+      <c r="C79" s="29"/>
+      <c r="D79" s="25">
+        <f t="shared" si="16"/>
         <v>210</v>
       </c>
-      <c r="E79" s="32"/>
-      <c r="F79" s="28">
-        <f>D79+ACTIVE2</f>
+      <c r="E79" s="29"/>
+      <c r="F79" s="25">
+        <f t="shared" si="17"/>
         <v>211</v>
       </c>
-      <c r="G79" s="32"/>
-      <c r="H79" s="28">
-        <f>F79+ACTIVE3</f>
+      <c r="G79" s="29"/>
+      <c r="H79" s="25">
+        <f t="shared" si="18"/>
         <v>212</v>
       </c>
-      <c r="I79" s="32"/>
+      <c r="I79" s="29"/>
     </row>
     <row r="80" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30">
+      <c r="A80" s="27">
         <v>54</v>
       </c>
-      <c r="B80" s="31">
-        <f>H79+ACTIVE4</f>
+      <c r="B80" s="28">
+        <f t="shared" si="19"/>
         <v>213</v>
       </c>
-      <c r="C80" s="32"/>
-      <c r="D80" s="28">
-        <f>B80+ACTIVE1</f>
+      <c r="C80" s="29"/>
+      <c r="D80" s="25">
+        <f t="shared" si="16"/>
         <v>214</v>
       </c>
-      <c r="E80" s="32"/>
-      <c r="F80" s="28">
-        <f>D80+ACTIVE2</f>
+      <c r="E80" s="29"/>
+      <c r="F80" s="25">
+        <f t="shared" si="17"/>
         <v>215</v>
       </c>
-      <c r="G80" s="32"/>
-      <c r="H80" s="28">
-        <f>F80+ACTIVE3</f>
+      <c r="G80" s="29"/>
+      <c r="H80" s="25">
+        <f t="shared" si="18"/>
         <v>216</v>
       </c>
-      <c r="I80" s="32"/>
+      <c r="I80" s="29"/>
     </row>
     <row r="81" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="27">
+      <c r="A81" s="24">
         <v>55</v>
       </c>
-      <c r="B81" s="31">
-        <f>H80+ACTIVE4</f>
+      <c r="B81" s="28">
+        <f t="shared" si="19"/>
         <v>217</v>
       </c>
-      <c r="C81" s="32"/>
-      <c r="D81" s="28">
-        <f>B81+ACTIVE1</f>
+      <c r="C81" s="29"/>
+      <c r="D81" s="25">
+        <f t="shared" si="16"/>
         <v>218</v>
       </c>
-      <c r="E81" s="32"/>
-      <c r="F81" s="28">
-        <f>D81+ACTIVE2</f>
+      <c r="E81" s="29"/>
+      <c r="F81" s="25">
+        <f t="shared" si="17"/>
         <v>219</v>
       </c>
-      <c r="G81" s="32"/>
-      <c r="H81" s="28">
-        <f>F81+ACTIVE3</f>
+      <c r="G81" s="29"/>
+      <c r="H81" s="25">
+        <f t="shared" si="18"/>
         <v>220</v>
       </c>
-      <c r="I81" s="32"/>
+      <c r="I81" s="29"/>
     </row>
     <row r="82" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="30">
+      <c r="A82" s="27">
         <v>56</v>
       </c>
-      <c r="B82" s="31">
-        <f>H81+ACTIVE4</f>
+      <c r="B82" s="28">
+        <f t="shared" si="19"/>
         <v>221</v>
       </c>
-      <c r="C82" s="32"/>
-      <c r="D82" s="28">
-        <f>B82+ACTIVE1</f>
+      <c r="C82" s="29"/>
+      <c r="D82" s="25">
+        <f t="shared" si="16"/>
         <v>222</v>
       </c>
-      <c r="E82" s="32"/>
-      <c r="F82" s="28">
-        <f>D82+ACTIVE2</f>
+      <c r="E82" s="29"/>
+      <c r="F82" s="25">
+        <f t="shared" si="17"/>
         <v>223</v>
       </c>
-      <c r="G82" s="32"/>
-      <c r="H82" s="28">
-        <f>F82+ACTIVE3</f>
+      <c r="G82" s="29"/>
+      <c r="H82" s="25">
+        <f t="shared" si="18"/>
         <v>224</v>
       </c>
-      <c r="I82" s="32"/>
+      <c r="I82" s="29"/>
     </row>
     <row r="83" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27">
+      <c r="A83" s="24">
         <v>57</v>
       </c>
-      <c r="B83" s="31">
-        <f>H82+ACTIVE4</f>
+      <c r="B83" s="28">
+        <f t="shared" si="19"/>
         <v>225</v>
       </c>
-      <c r="C83" s="32"/>
-      <c r="D83" s="28">
-        <f>B83+ACTIVE1</f>
+      <c r="C83" s="29"/>
+      <c r="D83" s="25">
+        <f t="shared" si="16"/>
         <v>226</v>
       </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="28">
-        <f>D83+ACTIVE2</f>
+      <c r="E83" s="29"/>
+      <c r="F83" s="25">
+        <f t="shared" si="17"/>
         <v>227</v>
       </c>
-      <c r="G83" s="32"/>
-      <c r="H83" s="28">
-        <f>F83+ACTIVE3</f>
+      <c r="G83" s="29"/>
+      <c r="H83" s="25">
+        <f t="shared" si="18"/>
         <v>228</v>
       </c>
-      <c r="I83" s="32"/>
+      <c r="I83" s="29"/>
     </row>
     <row r="84" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="30">
+      <c r="A84" s="27">
         <v>58</v>
       </c>
-      <c r="B84" s="31">
-        <f>H83+ACTIVE4</f>
+      <c r="B84" s="28">
+        <f t="shared" si="19"/>
         <v>229</v>
       </c>
-      <c r="C84" s="32"/>
-      <c r="D84" s="28">
-        <f>B84+ACTIVE1</f>
+      <c r="C84" s="29"/>
+      <c r="D84" s="25">
+        <f t="shared" si="16"/>
         <v>230</v>
       </c>
-      <c r="E84" s="32"/>
-      <c r="F84" s="28">
-        <f>D84+ACTIVE2</f>
+      <c r="E84" s="29"/>
+      <c r="F84" s="25">
+        <f t="shared" si="17"/>
         <v>231</v>
       </c>
-      <c r="G84" s="32"/>
-      <c r="H84" s="28">
-        <f>F84+ACTIVE3</f>
+      <c r="G84" s="29"/>
+      <c r="H84" s="25">
+        <f t="shared" si="18"/>
         <v>232</v>
       </c>
-      <c r="I84" s="32"/>
+      <c r="I84" s="29"/>
     </row>
     <row r="85" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="27">
+      <c r="A85" s="24">
         <v>59</v>
       </c>
-      <c r="B85" s="31">
-        <f>H84+ACTIVE4</f>
+      <c r="B85" s="28">
+        <f t="shared" si="19"/>
         <v>233</v>
       </c>
-      <c r="C85" s="32"/>
-      <c r="D85" s="28">
-        <f>B85+ACTIVE1</f>
+      <c r="C85" s="29"/>
+      <c r="D85" s="25">
+        <f t="shared" si="16"/>
         <v>234</v>
       </c>
-      <c r="E85" s="32"/>
-      <c r="F85" s="28">
-        <f>D85+ACTIVE2</f>
+      <c r="E85" s="29"/>
+      <c r="F85" s="25">
+        <f t="shared" si="17"/>
         <v>235</v>
       </c>
-      <c r="G85" s="32"/>
-      <c r="H85" s="28">
-        <f>F85+ACTIVE3</f>
+      <c r="G85" s="29"/>
+      <c r="H85" s="25">
+        <f t="shared" si="18"/>
         <v>236</v>
       </c>
-      <c r="I85" s="32"/>
+      <c r="I85" s="29"/>
     </row>
     <row r="86" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="33">
+      <c r="A86" s="30">
         <v>60</v>
       </c>
-      <c r="B86" s="34">
-        <f>H85+ACTIVE4</f>
+      <c r="B86" s="31">
+        <f t="shared" si="19"/>
         <v>237</v>
       </c>
-      <c r="C86" s="35"/>
-      <c r="D86" s="44">
-        <f>B86+ACTIVE1</f>
+      <c r="C86" s="32"/>
+      <c r="D86" s="41">
+        <f t="shared" si="16"/>
         <v>238</v>
       </c>
-      <c r="E86" s="35"/>
-      <c r="F86" s="44">
-        <f>D86+ACTIVE2</f>
+      <c r="E86" s="32"/>
+      <c r="F86" s="41">
+        <f t="shared" si="17"/>
         <v>239</v>
       </c>
-      <c r="G86" s="35"/>
-      <c r="H86" s="44">
-        <f>F86+ACTIVE3</f>
+      <c r="G86" s="32"/>
+      <c r="H86" s="41">
+        <f t="shared" si="18"/>
         <v>240</v>
       </c>
-      <c r="I86" s="35"/>
+      <c r="I86" s="32"/>
     </row>
     <row r="87" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H87" s="36" t="s">
+      <c r="H87" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I87" s="37">
+      <c r="I87" s="34">
         <f>SUMPRODUCT(LEN(C75:I86)-LEN(SUBSTITUTE(UPPER(C75:I86),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B88" s="23" t="s">
+      <c r="B88" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C88" s="24"/>
+      <c r="C88" s="21"/>
     </row>
     <row r="89" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C89" s="26" t="s">
+      <c r="C89" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D89" s="25" t="s">
+      <c r="D89" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E89" s="26" t="s">
+      <c r="E89" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="25" t="s">
+      <c r="F89" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G89" s="26" t="s">
+      <c r="G89" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H89" s="25" t="s">
+      <c r="H89" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I89" s="26" t="s">
+      <c r="I89" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="38">
+      <c r="A90" s="35">
         <v>61</v>
       </c>
-      <c r="B90" s="28">
+      <c r="B90" s="25">
         <f>H86+ACTIVE4</f>
         <v>241</v>
       </c>
-      <c r="C90" s="29"/>
-      <c r="D90" s="42">
-        <f>B90+ACTIVE1</f>
+      <c r="C90" s="26"/>
+      <c r="D90" s="39">
+        <f t="shared" ref="D90:D101" si="20">B90+ACTIVE1</f>
         <v>242</v>
       </c>
-      <c r="E90" s="29"/>
-      <c r="F90" s="42">
-        <f>D90+ACTIVE2</f>
+      <c r="E90" s="26"/>
+      <c r="F90" s="39">
+        <f t="shared" ref="F90:F101" si="21">D90+ACTIVE2</f>
         <v>243</v>
       </c>
-      <c r="G90" s="29"/>
-      <c r="H90" s="42">
-        <f>F90+ACTIVE3</f>
+      <c r="G90" s="26"/>
+      <c r="H90" s="39">
+        <f t="shared" ref="H90:H101" si="22">F90+ACTIVE3</f>
         <v>244</v>
       </c>
-      <c r="I90" s="29"/>
+      <c r="I90" s="26"/>
     </row>
     <row r="91" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="30">
+      <c r="A91" s="27">
         <v>62</v>
       </c>
-      <c r="B91" s="31">
-        <f>H90+ACTIVE4</f>
+      <c r="B91" s="28">
+        <f t="shared" ref="B91:B101" si="23">H90+ACTIVE4</f>
         <v>245</v>
       </c>
-      <c r="C91" s="32"/>
-      <c r="D91" s="28">
-        <f>B91+ACTIVE1</f>
+      <c r="C91" s="29"/>
+      <c r="D91" s="25">
+        <f t="shared" si="20"/>
         <v>246</v>
       </c>
-      <c r="E91" s="32"/>
-      <c r="F91" s="28">
-        <f>D91+ACTIVE2</f>
+      <c r="E91" s="29"/>
+      <c r="F91" s="25">
+        <f t="shared" si="21"/>
         <v>247</v>
       </c>
-      <c r="G91" s="32"/>
-      <c r="H91" s="28">
-        <f>F91+ACTIVE3</f>
+      <c r="G91" s="29"/>
+      <c r="H91" s="25">
+        <f t="shared" si="22"/>
         <v>248</v>
       </c>
-      <c r="I91" s="32"/>
+      <c r="I91" s="29"/>
     </row>
     <row r="92" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="27">
+      <c r="A92" s="24">
         <v>63</v>
       </c>
-      <c r="B92" s="31">
-        <f>H91+ACTIVE4</f>
+      <c r="B92" s="28">
+        <f t="shared" si="23"/>
         <v>249</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="28">
-        <f>B92+ACTIVE1</f>
+      <c r="C92" s="29"/>
+      <c r="D92" s="25">
+        <f t="shared" si="20"/>
         <v>250</v>
       </c>
-      <c r="E92" s="32"/>
-      <c r="F92" s="28">
-        <f>D92+ACTIVE2</f>
+      <c r="E92" s="29"/>
+      <c r="F92" s="25">
+        <f t="shared" si="21"/>
         <v>251</v>
       </c>
-      <c r="G92" s="32"/>
-      <c r="H92" s="28">
-        <f>F92+ACTIVE3</f>
+      <c r="G92" s="29"/>
+      <c r="H92" s="25">
+        <f t="shared" si="22"/>
         <v>252</v>
       </c>
-      <c r="I92" s="32"/>
+      <c r="I92" s="29"/>
     </row>
     <row r="93" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="30">
+      <c r="A93" s="27">
         <v>64</v>
       </c>
-      <c r="B93" s="31">
-        <f>H92+ACTIVE4</f>
+      <c r="B93" s="28">
+        <f t="shared" si="23"/>
         <v>253</v>
       </c>
-      <c r="C93" s="32"/>
-      <c r="D93" s="28">
-        <f>B93+ACTIVE1</f>
+      <c r="C93" s="29"/>
+      <c r="D93" s="25">
+        <f t="shared" si="20"/>
         <v>254</v>
       </c>
-      <c r="E93" s="32"/>
-      <c r="F93" s="28">
-        <f>D93+ACTIVE2</f>
+      <c r="E93" s="29"/>
+      <c r="F93" s="25">
+        <f t="shared" si="21"/>
         <v>255</v>
       </c>
-      <c r="G93" s="32"/>
-      <c r="H93" s="28">
-        <f>F93+ACTIVE3</f>
+      <c r="G93" s="29"/>
+      <c r="H93" s="25">
+        <f t="shared" si="22"/>
         <v>256</v>
       </c>
-      <c r="I93" s="32"/>
+      <c r="I93" s="29"/>
     </row>
     <row r="94" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="27">
+      <c r="A94" s="24">
         <v>65</v>
       </c>
-      <c r="B94" s="31">
-        <f>H93+ACTIVE4</f>
+      <c r="B94" s="28">
+        <f t="shared" si="23"/>
         <v>257</v>
       </c>
-      <c r="C94" s="32"/>
-      <c r="D94" s="28">
-        <f>B94+ACTIVE1</f>
+      <c r="C94" s="29"/>
+      <c r="D94" s="25">
+        <f t="shared" si="20"/>
         <v>258</v>
       </c>
-      <c r="E94" s="32"/>
-      <c r="F94" s="28">
-        <f>D94+ACTIVE2</f>
+      <c r="E94" s="29"/>
+      <c r="F94" s="25">
+        <f t="shared" si="21"/>
         <v>259</v>
       </c>
-      <c r="G94" s="32"/>
-      <c r="H94" s="28">
-        <f>F94+ACTIVE3</f>
+      <c r="G94" s="29"/>
+      <c r="H94" s="25">
+        <f t="shared" si="22"/>
         <v>260</v>
       </c>
-      <c r="I94" s="32"/>
+      <c r="I94" s="29"/>
     </row>
     <row r="95" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="30">
+      <c r="A95" s="27">
         <v>66</v>
       </c>
-      <c r="B95" s="31">
-        <f>H94+ACTIVE4</f>
+      <c r="B95" s="28">
+        <f t="shared" si="23"/>
         <v>261</v>
       </c>
-      <c r="C95" s="32"/>
-      <c r="D95" s="28">
-        <f>B95+ACTIVE1</f>
+      <c r="C95" s="29"/>
+      <c r="D95" s="25">
+        <f t="shared" si="20"/>
         <v>262</v>
       </c>
-      <c r="E95" s="32"/>
-      <c r="F95" s="28">
-        <f>D95+ACTIVE2</f>
+      <c r="E95" s="29"/>
+      <c r="F95" s="25">
+        <f t="shared" si="21"/>
         <v>263</v>
       </c>
-      <c r="G95" s="32"/>
-      <c r="H95" s="28">
-        <f>F95+ACTIVE3</f>
+      <c r="G95" s="29"/>
+      <c r="H95" s="25">
+        <f t="shared" si="22"/>
         <v>264</v>
       </c>
-      <c r="I95" s="32"/>
+      <c r="I95" s="29"/>
     </row>
     <row r="96" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="27">
+      <c r="A96" s="24">
         <v>67</v>
       </c>
-      <c r="B96" s="31">
-        <f>H95+ACTIVE4</f>
+      <c r="B96" s="28">
+        <f t="shared" si="23"/>
         <v>265</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="28">
-        <f>B96+ACTIVE1</f>
+      <c r="C96" s="29"/>
+      <c r="D96" s="25">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="E96" s="32"/>
-      <c r="F96" s="28">
-        <f>D96+ACTIVE2</f>
+      <c r="E96" s="29"/>
+      <c r="F96" s="25">
+        <f t="shared" si="21"/>
         <v>267</v>
       </c>
-      <c r="G96" s="32"/>
-      <c r="H96" s="28">
-        <f>F96+ACTIVE3</f>
+      <c r="G96" s="29"/>
+      <c r="H96" s="25">
+        <f t="shared" si="22"/>
         <v>268</v>
       </c>
-      <c r="I96" s="32"/>
+      <c r="I96" s="29"/>
     </row>
     <row r="97" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30">
+      <c r="A97" s="27">
         <v>68</v>
       </c>
-      <c r="B97" s="31">
-        <f>H96+ACTIVE4</f>
+      <c r="B97" s="28">
+        <f t="shared" si="23"/>
         <v>269</v>
       </c>
-      <c r="C97" s="32"/>
-      <c r="D97" s="28">
-        <f>B97+ACTIVE1</f>
+      <c r="C97" s="29"/>
+      <c r="D97" s="25">
+        <f t="shared" si="20"/>
         <v>270</v>
       </c>
-      <c r="E97" s="32"/>
-      <c r="F97" s="28">
-        <f>D97+ACTIVE2</f>
+      <c r="E97" s="29"/>
+      <c r="F97" s="25">
+        <f t="shared" si="21"/>
         <v>271</v>
       </c>
-      <c r="G97" s="32"/>
-      <c r="H97" s="28">
-        <f>F97+ACTIVE3</f>
+      <c r="G97" s="29"/>
+      <c r="H97" s="25">
+        <f t="shared" si="22"/>
         <v>272</v>
       </c>
-      <c r="I97" s="32"/>
+      <c r="I97" s="29"/>
     </row>
     <row r="98" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="27">
+      <c r="A98" s="24">
         <v>69</v>
       </c>
-      <c r="B98" s="31">
-        <f>H97+ACTIVE4</f>
+      <c r="B98" s="28">
+        <f t="shared" si="23"/>
         <v>273</v>
       </c>
-      <c r="C98" s="32"/>
-      <c r="D98" s="28">
-        <f>B98+ACTIVE1</f>
+      <c r="C98" s="29"/>
+      <c r="D98" s="25">
+        <f t="shared" si="20"/>
         <v>274</v>
       </c>
-      <c r="E98" s="32"/>
-      <c r="F98" s="28">
-        <f>D98+ACTIVE2</f>
+      <c r="E98" s="29"/>
+      <c r="F98" s="25">
+        <f t="shared" si="21"/>
         <v>275</v>
       </c>
-      <c r="G98" s="32"/>
-      <c r="H98" s="28">
-        <f>F98+ACTIVE3</f>
+      <c r="G98" s="29"/>
+      <c r="H98" s="25">
+        <f t="shared" si="22"/>
         <v>276</v>
       </c>
-      <c r="I98" s="32"/>
+      <c r="I98" s="29"/>
     </row>
     <row r="99" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30">
+      <c r="A99" s="27">
         <v>70</v>
       </c>
-      <c r="B99" s="31">
-        <f>H98+ACTIVE4</f>
+      <c r="B99" s="28">
+        <f t="shared" si="23"/>
         <v>277</v>
       </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="28">
-        <f>B99+ACTIVE1</f>
+      <c r="C99" s="29"/>
+      <c r="D99" s="25">
+        <f t="shared" si="20"/>
         <v>278</v>
       </c>
-      <c r="E99" s="32"/>
-      <c r="F99" s="28">
-        <f>D99+ACTIVE2</f>
+      <c r="E99" s="29"/>
+      <c r="F99" s="25">
+        <f t="shared" si="21"/>
         <v>279</v>
       </c>
-      <c r="G99" s="32"/>
-      <c r="H99" s="28">
-        <f>F99+ACTIVE3</f>
+      <c r="G99" s="29"/>
+      <c r="H99" s="25">
+        <f t="shared" si="22"/>
         <v>280</v>
       </c>
-      <c r="I99" s="32"/>
+      <c r="I99" s="29"/>
     </row>
     <row r="100" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="27">
+      <c r="A100" s="24">
         <v>71</v>
       </c>
-      <c r="B100" s="31">
-        <f>H99+ACTIVE4</f>
+      <c r="B100" s="28">
+        <f t="shared" si="23"/>
         <v>281</v>
       </c>
-      <c r="C100" s="32"/>
-      <c r="D100" s="28">
-        <f>B100+ACTIVE1</f>
+      <c r="C100" s="29"/>
+      <c r="D100" s="25">
+        <f t="shared" si="20"/>
         <v>282</v>
       </c>
-      <c r="E100" s="32"/>
-      <c r="F100" s="28">
-        <f>D100+ACTIVE2</f>
+      <c r="E100" s="29"/>
+      <c r="F100" s="25">
+        <f t="shared" si="21"/>
         <v>283</v>
       </c>
-      <c r="G100" s="32"/>
-      <c r="H100" s="28">
-        <f>F100+ACTIVE3</f>
+      <c r="G100" s="29"/>
+      <c r="H100" s="25">
+        <f t="shared" si="22"/>
         <v>284</v>
       </c>
-      <c r="I100" s="32"/>
+      <c r="I100" s="29"/>
     </row>
     <row r="101" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="33">
+      <c r="A101" s="30">
         <v>72</v>
       </c>
-      <c r="B101" s="34">
-        <f>H100+ACTIVE4</f>
+      <c r="B101" s="31">
+        <f t="shared" si="23"/>
         <v>285</v>
       </c>
-      <c r="C101" s="35"/>
-      <c r="D101" s="44">
-        <f>B101+ACTIVE1</f>
+      <c r="C101" s="32"/>
+      <c r="D101" s="41">
+        <f t="shared" si="20"/>
         <v>286</v>
       </c>
-      <c r="E101" s="35"/>
-      <c r="F101" s="44">
-        <f>D101+ACTIVE2</f>
+      <c r="E101" s="32"/>
+      <c r="F101" s="41">
+        <f t="shared" si="21"/>
         <v>287</v>
       </c>
-      <c r="G101" s="35"/>
-      <c r="H101" s="44">
-        <f>F101+ACTIVE3</f>
+      <c r="G101" s="32"/>
+      <c r="H101" s="41">
+        <f t="shared" si="22"/>
         <v>288</v>
       </c>
-      <c r="I101" s="35"/>
+      <c r="I101" s="32"/>
     </row>
     <row r="102" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H102" s="36" t="s">
+      <c r="H102" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I102" s="37">
+      <c r="I102" s="34">
         <f>SUMPRODUCT(LEN(C90:I101)-LEN(SUBSTITUTE(UPPER(C90:I101),"X","")))</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="39" t="s">
+      <c r="B106" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B107" s="39" t="s">
+      <c r="B107" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="39" t="s">
+      <c r="B108" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E114" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4349,92 +4510,92 @@
     <mergeCell ref="B7:C7"/>
   </mergeCells>
   <conditionalFormatting sqref="I30:I41 I15:I26">
-    <cfRule type="expression" dxfId="65" priority="49">
+    <cfRule type="expression" dxfId="41" priority="49">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:C26 B30:C41">
-    <cfRule type="expression" dxfId="64" priority="50">
+    <cfRule type="expression" dxfId="40" priority="50">
       <formula>SUBJECT1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:E26 D30:E41">
-    <cfRule type="expression" dxfId="63" priority="51">
+    <cfRule type="expression" dxfId="39" priority="51">
       <formula>SUBJECT2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G41 G15:G26">
-    <cfRule type="expression" dxfId="62" priority="52">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G41 G15:G26">
-    <cfRule type="expression" dxfId="51" priority="47">
+    <cfRule type="expression" dxfId="37" priority="47">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I41 I15:I26">
-    <cfRule type="expression" dxfId="50" priority="45">
+    <cfRule type="expression" dxfId="36" priority="45">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F26">
-    <cfRule type="expression" dxfId="49" priority="44">
+    <cfRule type="expression" dxfId="35" priority="44">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H26">
-    <cfRule type="expression" dxfId="48" priority="43">
+    <cfRule type="expression" dxfId="34" priority="43">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:F41">
-    <cfRule type="expression" dxfId="47" priority="42">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H41">
-    <cfRule type="expression" dxfId="46" priority="41">
+    <cfRule type="expression" dxfId="32" priority="41">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:I56">
-    <cfRule type="expression" dxfId="39" priority="37">
+    <cfRule type="expression" dxfId="31" priority="37">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:C56">
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="30" priority="38">
       <formula>SUBJECT1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:E56">
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>SUBJECT2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:G56">
-    <cfRule type="expression" dxfId="36" priority="40">
+    <cfRule type="expression" dxfId="28" priority="40">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:G56">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:I56">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="26" priority="35">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:F56">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="25" priority="34">
       <formula>SUBJECT3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:H56">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="24" priority="33">
       <formula>SUBJECT4=""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>